<commit_message>
feature: updaed all excel sheets
</commit_message>
<xml_diff>
--- a/src/final/inner_prediction/inner_cross_pred_results.xlsx
+++ b/src/final/inner_prediction/inner_cross_pred_results.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
-    <sheet name="NN (v)" sheetId="4" r:id="rId1"/>
-    <sheet name="NN (u)" sheetId="5" r:id="rId2"/>
-    <sheet name="NN (Trainlength)" sheetId="12" r:id="rId3"/>
-    <sheet name="RBF (v)" sheetId="8" r:id="rId4"/>
-    <sheet name="RBF (u)" sheetId="10" r:id="rId5"/>
-    <sheet name="ESN (v)" sheetId="13" r:id="rId6"/>
-    <sheet name="ESN (u)" sheetId="15" r:id="rId7"/>
-    <sheet name="Default Errors" sheetId="16" r:id="rId8"/>
+    <sheet name="Summary" sheetId="17" r:id="rId1"/>
+    <sheet name="NN (v)" sheetId="4" r:id="rId2"/>
+    <sheet name="NN (u)" sheetId="5" r:id="rId3"/>
+    <sheet name="NN (Trainlength)" sheetId="12" r:id="rId4"/>
+    <sheet name="RBF (v)" sheetId="8" r:id="rId5"/>
+    <sheet name="RBF (u)" sheetId="10" r:id="rId6"/>
+    <sheet name="ESN (v)" sheetId="13" r:id="rId7"/>
+    <sheet name="ESN (u)" sheetId="15" r:id="rId8"/>
+    <sheet name="Default Errors" sheetId="16" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="42">
   <si>
     <t>MSE</t>
   </si>
@@ -146,6 +147,18 @@
   <si>
     <t>mse (mean)</t>
   </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>Best</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>(64x64)</t>
+  </si>
 </sst>
 </file>
 
@@ -155,7 +168,7 @@
     <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
     <numFmt numFmtId="165" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +251,14 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -303,7 +324,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -348,6 +369,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Ausgabe" xfId="2" builtinId="21"/>
@@ -3059,10 +3081,410 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:L16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="9" max="12" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B5" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <f>'NN (v)'!B$12</f>
+        <v>15000</v>
+      </c>
+      <c r="E6" s="1">
+        <f>'NN (v)'!C$12</f>
+        <v>64</v>
+      </c>
+      <c r="F6" s="1">
+        <f>'NN (v)'!D$12</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="19">
+        <f>'NN (v)'!G$12</f>
+        <v>0.23462962962962963</v>
+      </c>
+      <c r="H6" s="25">
+        <f>'NN (v)'!H$12</f>
+        <v>9.28317864542402E-2</v>
+      </c>
+      <c r="I6" s="9">
+        <f>'NN (v)'!K$12</f>
+        <v>1.4011911255298943</v>
+      </c>
+      <c r="J6" s="9">
+        <f>'NN (v)'!L$12</f>
+        <v>1.1837191920087695</v>
+      </c>
+      <c r="K6" s="9">
+        <f>'NN (v)'!M$12</f>
+        <v>1.3784834237012626</v>
+      </c>
+      <c r="L6" s="9">
+        <f>'NN (v)'!N$12</f>
+        <v>1.174088337264817</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <f>'RBF (v)'!B$12</f>
+        <v>15000</v>
+      </c>
+      <c r="E7" s="1">
+        <f>'RBF (v)'!C$12</f>
+        <v>64</v>
+      </c>
+      <c r="F7" s="1">
+        <f>'RBF (v)'!D$12</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="19">
+        <f>'RBF (v)'!G$12</f>
+        <v>2.0324074074074074E-2</v>
+      </c>
+      <c r="H7" s="25">
+        <f>'RBF (v)'!H$12</f>
+        <v>5.5880421850485799E-2</v>
+      </c>
+      <c r="I7" s="9">
+        <f>'RBF (v)'!K$12</f>
+        <v>0.84345194871762685</v>
+      </c>
+      <c r="J7" s="9">
+        <f>'RBF (v)'!L$12</f>
+        <v>0.91839640064496486</v>
+      </c>
+      <c r="K7" s="9">
+        <f>'RBF (v)'!M$12</f>
+        <v>0.82978296737076385</v>
+      </c>
+      <c r="L7" s="9">
+        <f>'RBF (v)'!N$12</f>
+        <v>0.91092423799719147</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <f>'ESN (v)'!B$12</f>
+        <v>15000</v>
+      </c>
+      <c r="E8" s="1">
+        <f>'ESN (v)'!C$12</f>
+        <v>64</v>
+      </c>
+      <c r="F8" s="1">
+        <f>'ESN (v)'!D$12</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="19">
+        <f>'ESN (v)'!L$12</f>
+        <v>4.4212962962962956E-3</v>
+      </c>
+      <c r="H8" s="25">
+        <f>'ESN (v)'!M$12</f>
+        <v>0.104995827502257</v>
+      </c>
+      <c r="I8" s="9">
+        <f>'ESN (v)'!P$12</f>
+        <v>1.5847936071590085</v>
+      </c>
+      <c r="J8" s="9">
+        <f>'ESN (v)'!Q$12</f>
+        <v>1.2588858594642363</v>
+      </c>
+      <c r="K8" s="9">
+        <f>'ESN (v)'!R$12</f>
+        <v>1.5591104437164203</v>
+      </c>
+      <c r="L8" s="9">
+        <f>'ESN (v)'!S$12</f>
+        <v>1.248643441386059</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="7" t="str">
+        <f>INDEX(C6:C8,MATCH(MIN($H$6:$H$8),$H$6:$H$8,))</f>
+        <v>RBF</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" ref="D9:L9" si="0">INDEX(D6:D8,MATCH(MIN($H$6:$H$8),$H$6:$H$8,))</f>
+        <v>15000</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="20">
+        <f t="shared" si="0"/>
+        <v>2.0324074074074074E-2</v>
+      </c>
+      <c r="H9" s="7">
+        <f t="shared" si="0"/>
+        <v>5.5880421850485799E-2</v>
+      </c>
+      <c r="I9" s="26">
+        <f t="shared" si="0"/>
+        <v>0.84345194871762685</v>
+      </c>
+      <c r="J9" s="26">
+        <f t="shared" si="0"/>
+        <v>0.91839640064496486</v>
+      </c>
+      <c r="K9" s="26">
+        <f t="shared" si="0"/>
+        <v>0.82978296737076385</v>
+      </c>
+      <c r="L9" s="26">
+        <f t="shared" si="0"/>
+        <v>0.91092423799719147</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B12" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1">
+        <f>'NN (u)'!B$12</f>
+        <v>15000</v>
+      </c>
+      <c r="E13" s="1">
+        <f>'NN (u)'!C$12</f>
+        <v>64</v>
+      </c>
+      <c r="F13" s="1">
+        <f>'NN (u)'!D$12</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="19">
+        <f>'NN (u)'!G$12</f>
+        <v>0.17076388888888891</v>
+      </c>
+      <c r="H13" s="25">
+        <f>'NN (u)'!H$12</f>
+        <v>0.24599091371974699</v>
+      </c>
+      <c r="I13" s="9">
+        <f>'NN (u)'!I$12</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="9">
+        <f>'NN (u)'!J$12</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="9">
+        <f>'NN (u)'!K$12</f>
+        <v>1.7008816745909097</v>
+      </c>
+      <c r="L13" s="9">
+        <f>'NN (u)'!L$12</f>
+        <v>1.3041785439850289</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1">
+        <f>'RBF (u)'!B$12</f>
+        <v>15000</v>
+      </c>
+      <c r="E14" s="1">
+        <f>'RBF (u)'!C$12</f>
+        <v>64</v>
+      </c>
+      <c r="F14" s="1">
+        <f>'RBF (u)'!D$12</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="19">
+        <f>'RBF (u)'!G$12</f>
+        <v>2.1354166666666664E-2</v>
+      </c>
+      <c r="H14" s="25">
+        <f>'RBF (u)'!H$12</f>
+        <v>0.136152908081632</v>
+      </c>
+      <c r="I14" s="9">
+        <f>'RBF (u)'!I$12</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="9">
+        <f>'RBF (u)'!J$12</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="9">
+        <f>'RBF (u)'!K$12</f>
+        <v>0.94141683038806601</v>
+      </c>
+      <c r="L14" s="9">
+        <f>'RBF (u)'!L$12</f>
+        <v>0.97026637084259804</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
+        <f>'ESN (u)'!B$12</f>
+        <v>15000</v>
+      </c>
+      <c r="E15" s="1">
+        <f>'ESN (u)'!C$12</f>
+        <v>64</v>
+      </c>
+      <c r="F15" s="1">
+        <f>'ESN (u)'!D$12</f>
+        <v>3</v>
+      </c>
+      <c r="G15" s="19">
+        <f>'ESN (u)'!L$12</f>
+        <v>4.4907407407407405E-3</v>
+      </c>
+      <c r="H15" s="25">
+        <f>'ESN (u)'!M$12</f>
+        <v>0.146226345122142</v>
+      </c>
+      <c r="I15" s="9">
+        <f>'ESN (u)'!N$12</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="9">
+        <f>'ESN (u)'!O$12</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="9">
+        <f>'ESN (u)'!P$12</f>
+        <v>1.0110686894883125</v>
+      </c>
+      <c r="L15" s="9">
+        <f>'ESN (u)'!Q$12</f>
+        <v>1.005519114432099</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="7" t="str">
+        <f>INDEX(C13:C15,MATCH(MIN($H$6:$H$8),$H$6:$H$8,))</f>
+        <v>RBF</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" ref="D16:L16" si="1">INDEX(D13:D15,MATCH(MIN($H$6:$H$8),$H$6:$H$8,))</f>
+        <v>15000</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="F16" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G16" s="20">
+        <f t="shared" si="1"/>
+        <v>2.1354166666666664E-2</v>
+      </c>
+      <c r="H16" s="7">
+        <f t="shared" si="1"/>
+        <v>0.136152908081632</v>
+      </c>
+      <c r="I16" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="26">
+        <f t="shared" si="1"/>
+        <v>0.94141683038806601</v>
+      </c>
+      <c r="L16" s="26">
+        <f t="shared" si="1"/>
+        <v>0.97026637084259804</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="B13" sqref="B13:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7899,7 +8321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O105"/>
   <sheetViews>
@@ -12565,7 +12987,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M30"/>
   <sheetViews>
@@ -13102,12 +13524,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R291"/>
   <sheetViews>
-    <sheetView topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27505,11 +27927,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AA291"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:B12"/>
     </sheetView>
   </sheetViews>
@@ -43922,11 +44344,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P15" sqref="P11:P15"/>
     </sheetView>
   </sheetViews>
@@ -46093,7 +46515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:U84"/>
   <sheetViews>
@@ -48278,7 +48700,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:L27"/>
   <sheetViews>

</xml_diff>

<commit_message>
feature: added new results for broader grid search for inner cross prediction
</commit_message>
<xml_diff>
--- a/src/final/inner_prediction/inner_cross_pred_results.xlsx
+++ b/src/final/inner_prediction/inner_cross_pred_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="17" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="45">
   <si>
     <t>MSE</t>
   </si>
@@ -158,6 +158,15 @@
   </si>
   <si>
     <t>(64x64)</t>
+  </si>
+  <si>
+    <t>Optimized</t>
+  </si>
+  <si>
+    <t>5-O</t>
+  </si>
+  <si>
+    <t>New results</t>
   </si>
 </sst>
 </file>
@@ -360,6 +369,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="7" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -369,7 +379,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Ausgabe" xfId="2" builtinId="21"/>
@@ -3083,8 +3092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3123,10 +3132,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="27" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3230,27 +3239,27 @@
       </c>
       <c r="G8" s="19">
         <f>'ESN (v)'!L$12</f>
-        <v>4.4212962962962956E-3</v>
+        <v>1.2604166666666666E-2</v>
       </c>
       <c r="H8" s="25">
         <f>'ESN (v)'!M$12</f>
-        <v>0.104995827502257</v>
+        <v>5.3888242223566203E-2</v>
       </c>
       <c r="I8" s="9">
         <f>'ESN (v)'!P$12</f>
-        <v>1.5847936071590085</v>
+        <v>0.81338224392877012</v>
       </c>
       <c r="J8" s="9">
         <f>'ESN (v)'!Q$12</f>
-        <v>1.2588858594642363</v>
+        <v>0.90187706697130854</v>
       </c>
       <c r="K8" s="9">
         <f>'ESN (v)'!R$12</f>
-        <v>1.5591104437164203</v>
+        <v>0.80020057218441554</v>
       </c>
       <c r="L8" s="9">
         <f>'ESN (v)'!S$12</f>
-        <v>1.248643441386059</v>
+        <v>0.89453930723273167</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="16.5" x14ac:dyDescent="0.3">
@@ -3259,7 +3268,7 @@
       </c>
       <c r="C9" s="7" t="str">
         <f>INDEX(C6:C8,MATCH(MIN($H$6:$H$8),$H$6:$H$8,))</f>
-        <v>RBF</v>
+        <v>ESN</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" ref="D9:L9" si="0">INDEX(D6:D8,MATCH(MIN($H$6:$H$8),$H$6:$H$8,))</f>
@@ -3275,34 +3284,34 @@
       </c>
       <c r="G9" s="20">
         <f t="shared" si="0"/>
-        <v>2.0324074074074074E-2</v>
+        <v>1.2604166666666666E-2</v>
       </c>
       <c r="H9" s="7">
         <f t="shared" si="0"/>
-        <v>5.5880421850485799E-2</v>
+        <v>5.3888242223566203E-2</v>
       </c>
       <c r="I9" s="26">
         <f t="shared" si="0"/>
-        <v>0.84345194871762685</v>
+        <v>0.81338224392877012</v>
       </c>
       <c r="J9" s="26">
         <f t="shared" si="0"/>
-        <v>0.91839640064496486</v>
+        <v>0.90187706697130854</v>
       </c>
       <c r="K9" s="26">
         <f t="shared" si="0"/>
-        <v>0.82978296737076385</v>
+        <v>0.80020057218441554</v>
       </c>
       <c r="L9" s="26">
         <f t="shared" si="0"/>
-        <v>0.91092423799719147</v>
+        <v>0.89453930723273167</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="27" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3402,15 +3411,15 @@
       </c>
       <c r="F15" s="1">
         <f>'ESN (u)'!D$12</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G15" s="19">
         <f>'ESN (u)'!L$12</f>
-        <v>4.4907407407407405E-3</v>
+        <v>1.3958333333333335E-2</v>
       </c>
       <c r="H15" s="25">
         <f>'ESN (u)'!M$12</f>
-        <v>0.146226345122142</v>
+        <v>0.129747710464202</v>
       </c>
       <c r="I15" s="9">
         <f>'ESN (u)'!N$12</f>
@@ -3422,11 +3431,11 @@
       </c>
       <c r="K15" s="9">
         <f>'ESN (u)'!P$12</f>
-        <v>1.0110686894883125</v>
+        <v>0.89712867728159829</v>
       </c>
       <c r="L15" s="9">
         <f>'ESN (u)'!Q$12</f>
-        <v>1.005519114432099</v>
+        <v>0.94716876916503023</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="16.5" x14ac:dyDescent="0.3">
@@ -3435,7 +3444,7 @@
       </c>
       <c r="C16" s="7" t="str">
         <f>INDEX(C13:C15,MATCH(MIN($H$6:$H$8),$H$6:$H$8,))</f>
-        <v>RBF</v>
+        <v>ESN</v>
       </c>
       <c r="D16" s="7">
         <f t="shared" ref="D16:L16" si="1">INDEX(D13:D15,MATCH(MIN($H$6:$H$8),$H$6:$H$8,))</f>
@@ -3451,11 +3460,11 @@
       </c>
       <c r="G16" s="20">
         <f t="shared" si="1"/>
-        <v>2.1354166666666664E-2</v>
+        <v>1.3958333333333335E-2</v>
       </c>
       <c r="H16" s="7">
         <f t="shared" si="1"/>
-        <v>0.136152908081632</v>
+        <v>0.129747710464202</v>
       </c>
       <c r="I16" s="26">
         <f t="shared" si="1"/>
@@ -3467,11 +3476,11 @@
       </c>
       <c r="K16" s="26">
         <f t="shared" si="1"/>
-        <v>0.94141683038806601</v>
+        <v>0.89712867728159829</v>
       </c>
       <c r="L16" s="26">
         <f t="shared" si="1"/>
-        <v>0.97026637084259804</v>
+        <v>0.94716876916503023</v>
       </c>
     </row>
   </sheetData>
@@ -3483,7 +3492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B13" sqref="B13:N13"/>
     </sheetView>
   </sheetViews>
@@ -3519,14 +3528,14 @@
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
       <c r="K6" s="17"/>
@@ -8361,14 +8370,14 @@
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
       <c r="K6" s="6"/>
@@ -13015,11 +13024,11 @@
       <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
@@ -13562,14 +13571,14 @@
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
       <c r="K6" s="6"/>
@@ -27966,14 +27975,14 @@
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
       <c r="K6" s="6"/>
@@ -44348,8 +44357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P15" sqref="P11:P15"/>
+    <sheetView topLeftCell="H43" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46:M66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44387,17 +44396,17 @@
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
       <c r="N6" s="18"/>
       <c r="O6" s="18"/>
       <c r="P6" s="17"/>
@@ -44407,6 +44416,10 @@
       <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <f>INDEX(A$17:A$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,4),$M$17:$M$999,))</f>
+        <v>1</v>
+      </c>
       <c r="B8" s="7">
         <f>INDEX(B$17:B$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,4),$M$17:$M$999,))</f>
         <v>15000</v>
@@ -44421,11 +44434,11 @@
       </c>
       <c r="E8" s="7">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>400</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>1.5</v>
       </c>
       <c r="G8" s="7">
         <f t="shared" si="0"/>
@@ -44433,7 +44446,7 @@
       </c>
       <c r="H8" s="7">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I8" s="7">
         <f t="shared" si="0"/>
@@ -44441,40 +44454,44 @@
       </c>
       <c r="J8" s="7">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>1E-4</v>
       </c>
       <c r="K8" s="7">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="L8" s="20">
         <f t="shared" si="0"/>
-        <v>3.4722222222222222E-5</v>
+        <v>5.7870370370370366E-5</v>
       </c>
       <c r="M8" s="7">
         <f t="shared" si="0"/>
-        <v>3.2432352882883202E-4</v>
+        <v>2.5193958081904099E-4</v>
       </c>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="26">
         <f t="shared" si="0"/>
-        <v>6.0730353953692287E-3</v>
+        <v>4.7176287127044343E-3</v>
       </c>
       <c r="Q8" s="26">
         <f t="shared" si="0"/>
-        <v>7.7929682376930223E-2</v>
+        <v>6.8684996270688067E-2</v>
       </c>
       <c r="R8" s="26">
         <f t="shared" si="0"/>
-        <v>2.4008460894761562E-2</v>
+        <v>1.8650147264304324E-2</v>
       </c>
       <c r="S8" s="26">
         <f t="shared" si="0"/>
-        <v>0.15494663886242116</v>
+        <v>0.13656554200933824</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <f>INDEX(A$17:A$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,8),$M$17:$M$999,))</f>
+        <v>2</v>
+      </c>
       <c r="B9" s="7">
         <f>INDEX(B$17:B$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,8),$M$17:$M$999,))</f>
         <v>15000</v>
@@ -44543,6 +44560,10 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <f>INDEX(A$17:A$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,16),$M$17:$M$999,))</f>
+        <v>9</v>
+      </c>
       <c r="B10" s="7">
         <f>INDEX(B$17:B$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,16),$M$17:$M$999,))</f>
         <v>15000</v>
@@ -44553,7 +44574,7 @@
       </c>
       <c r="D10" s="7">
         <f t="shared" ref="D10:S10" si="2">INDEX(D$17:D$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,16),$M$17:$M$999,))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="2"/>
@@ -44581,7 +44602,7 @@
       </c>
       <c r="K10" s="7">
         <f t="shared" si="2"/>
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="L10" s="20">
         <f t="shared" si="2"/>
@@ -44589,28 +44610,32 @@
       </c>
       <c r="M10" s="7">
         <f t="shared" si="2"/>
-        <v>2.1032775498826799E-2</v>
+        <v>1.88640143419549E-2</v>
       </c>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
       <c r="P10" s="26">
         <f t="shared" si="2"/>
-        <v>0.31831235453262624</v>
+        <v>0.28549008291653333</v>
       </c>
       <c r="Q10" s="26">
         <f t="shared" si="2"/>
-        <v>0.56419177106071494</v>
+        <v>0.53431272015228437</v>
       </c>
       <c r="R10" s="26">
         <f t="shared" si="2"/>
-        <v>0.44568103720623981</v>
+        <v>0.39972534667451765</v>
       </c>
       <c r="S10" s="26">
         <f t="shared" si="2"/>
-        <v>0.66759346701884359</v>
+        <v>0.63223836222940288</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <f>INDEX(A$17:A$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,32),$M$17:$M$999,))</f>
+        <v>4</v>
+      </c>
       <c r="B11" s="7">
         <f>INDEX(B$17:B$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,32),$M$17:$M$999,))</f>
         <v>15000</v>
@@ -44625,19 +44650,19 @@
       </c>
       <c r="E11" s="7">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="G11" s="7">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.95</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" si="3"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" si="3"/>
@@ -44645,40 +44670,44 @@
       </c>
       <c r="J11" s="7">
         <f t="shared" si="3"/>
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" si="3"/>
-        <v>5.0000000000000001E-3</v>
+        <v>5000</v>
       </c>
       <c r="L11" s="20">
         <f t="shared" si="3"/>
-        <v>1.4004629629629629E-3</v>
+        <v>1.0532407407407407E-3</v>
       </c>
       <c r="M11" s="7">
         <f t="shared" si="3"/>
-        <v>9.0667343242407897E-2</v>
+        <v>4.23995426636763E-2</v>
       </c>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="26">
         <f t="shared" si="3"/>
-        <v>1.4063996828060041</v>
+        <v>0.657686673291899</v>
       </c>
       <c r="Q11" s="26">
         <f t="shared" si="3"/>
-        <v>1.1859172326962806</v>
+        <v>0.81097883652528135</v>
       </c>
       <c r="R11" s="26">
         <f t="shared" si="3"/>
-        <v>1.4800056032550533</v>
+        <v>0.69210763736531078</v>
       </c>
       <c r="S11" s="26">
         <f t="shared" si="3"/>
-        <v>1.2165548089811051</v>
+        <v>0.83193006759301036</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <f>INDEX(A$17:A$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,64),$M$17:$M$999,))</f>
+        <v>5</v>
+      </c>
       <c r="B12" s="7">
         <f>INDEX(B$17:B$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,64),$M$17:$M$999,))</f>
         <v>15000</v>
@@ -44693,11 +44722,11 @@
       </c>
       <c r="E12" s="7">
         <f t="shared" si="4"/>
-        <v>50</v>
+        <v>400</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="4"/>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="G12" s="7">
         <f t="shared" si="4"/>
@@ -44705,48 +44734,52 @@
       </c>
       <c r="H12" s="7">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I12" s="7">
         <f t="shared" si="4"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J12" s="7">
         <f t="shared" si="4"/>
-        <v>1.0000000000000001E-5</v>
+        <v>1E-4</v>
       </c>
       <c r="K12" s="7">
         <f t="shared" si="4"/>
-        <v>5.0000000000000001E-3</v>
+        <v>5000</v>
       </c>
       <c r="L12" s="20">
         <f t="shared" si="4"/>
-        <v>4.4212962962962956E-3</v>
+        <v>1.2604166666666666E-2</v>
       </c>
       <c r="M12" s="7">
         <f t="shared" si="4"/>
-        <v>0.104995827502257</v>
+        <v>5.3888242223566203E-2</v>
       </c>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
       <c r="P12" s="26">
         <f t="shared" si="4"/>
-        <v>1.5847936071590085</v>
+        <v>0.81338224392877012</v>
       </c>
       <c r="Q12" s="26">
         <f t="shared" si="4"/>
-        <v>1.2588858594642363</v>
+        <v>0.90187706697130854</v>
       </c>
       <c r="R12" s="26">
         <f t="shared" si="4"/>
-        <v>1.5591104437164203</v>
+        <v>0.80020057218441554</v>
       </c>
       <c r="S12" s="26">
         <f t="shared" si="4"/>
-        <v>1.248643441386059</v>
+        <v>0.89453930723273167</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <f>INDEX(A$17:A$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,128),$M$17:$M$999,))</f>
+        <v>6</v>
+      </c>
       <c r="B13" s="7">
         <f>INDEX(B$17:B$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,128),$M$17:$M$999,))</f>
         <v>15000</v>
@@ -44757,23 +44790,23 @@
       </c>
       <c r="D13" s="7">
         <f t="shared" ref="D13:S13" si="5">INDEX(D$17:D$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,128),$M$17:$M$999,))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="7">
         <f t="shared" si="5"/>
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="5"/>
-        <v>0.8</v>
+        <v>3</v>
       </c>
       <c r="G13" s="7">
         <f t="shared" si="5"/>
-        <v>0.95</v>
+        <v>0.05</v>
       </c>
       <c r="H13" s="7">
         <f t="shared" si="5"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I13" s="7">
         <f t="shared" si="5"/>
@@ -44785,36 +44818,40 @@
       </c>
       <c r="K13" s="7">
         <f t="shared" si="5"/>
-        <v>0.05</v>
+        <v>50000</v>
       </c>
       <c r="L13" s="20">
         <f t="shared" si="5"/>
-        <v>2.4062500000000001E-2</v>
+        <v>3.8599537037037036E-2</v>
       </c>
       <c r="M13" s="7">
         <f t="shared" si="5"/>
-        <v>0.11783850800270999</v>
+        <v>6.5956359710807794E-2</v>
       </c>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
       <c r="P13" s="26">
         <f t="shared" si="5"/>
-        <v>1.7799284979470402</v>
+        <v>0.99625840703459123</v>
       </c>
       <c r="Q13" s="26">
         <f t="shared" si="5"/>
-        <v>1.334139609616265</v>
+        <v>0.99812745029609884</v>
       </c>
       <c r="R13" s="26">
         <f t="shared" si="5"/>
-        <v>1.7651364797474716</v>
+        <v>0.98797904496733624</v>
       </c>
       <c r="S13" s="26">
         <f t="shared" si="5"/>
-        <v>1.3285843893962745</v>
+        <v>0.99397135017430771</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <f>INDEX(A$17:A$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,146),$M$17:$M$999,))</f>
+        <v>19</v>
+      </c>
       <c r="B14" s="7">
         <f>INDEX(B$17:B$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,146),$M$17:$M$999,))</f>
         <v>15000</v>
@@ -44837,7 +44874,7 @@
       </c>
       <c r="G14" s="7">
         <f t="shared" si="6"/>
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="H14" s="7">
         <f t="shared" si="6"/>
@@ -44845,7 +44882,7 @@
       </c>
       <c r="I14" s="7">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J14" s="7">
         <f t="shared" si="6"/>
@@ -44853,36 +44890,40 @@
       </c>
       <c r="K14" s="7">
         <f t="shared" si="6"/>
-        <v>0.05</v>
+        <v>50000</v>
       </c>
       <c r="L14" s="20">
         <f t="shared" si="6"/>
-        <v>5.4004629629629632E-2</v>
+        <v>5.3275462962962962E-2</v>
       </c>
       <c r="M14" s="7">
         <f t="shared" si="6"/>
-        <v>0.111810870933667</v>
+        <v>6.5437954795161096E-2</v>
       </c>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="26">
         <f t="shared" si="6"/>
-        <v>1.67562883370923</v>
+        <v>0.98067140482953563</v>
       </c>
       <c r="Q14" s="26">
         <f t="shared" si="6"/>
-        <v>1.2944608274139584</v>
+        <v>0.99028854624777707</v>
       </c>
       <c r="R14" s="26">
         <f t="shared" si="6"/>
-        <v>1.5578179721618732</v>
+        <v>0.91172192104554339</v>
       </c>
       <c r="S14" s="26">
         <f t="shared" si="6"/>
-        <v>1.2481257837901889</v>
+        <v>0.95484130673402656</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <f>INDEX(A$17:A$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,148),$M$17:$M$999,))</f>
+        <v>21</v>
+      </c>
       <c r="B15" s="7">
         <f>INDEX(B$17:B$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,148),$M$17:$M$999,))</f>
         <v>15000</v>
@@ -44901,7 +44942,7 @@
       </c>
       <c r="F15" s="7">
         <f t="shared" si="7"/>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="7"/>
@@ -44909,7 +44950,7 @@
       </c>
       <c r="H15" s="7">
         <f t="shared" si="7"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I15" s="7">
         <f t="shared" si="7"/>
@@ -44917,37 +44958,37 @@
       </c>
       <c r="J15" s="7">
         <f t="shared" si="7"/>
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K15" s="7">
         <f t="shared" si="7"/>
-        <v>0.05</v>
+        <v>50000</v>
       </c>
       <c r="L15" s="20">
         <f t="shared" si="7"/>
-        <v>5.5046296296296295E-2</v>
+        <v>5.4479166666666669E-2</v>
       </c>
       <c r="M15" s="7">
         <f t="shared" si="7"/>
-        <v>0.12718924615515101</v>
+        <v>6.4880812799093399E-2</v>
       </c>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="26">
         <f t="shared" si="7"/>
-        <v>1.8997822152911534</v>
+        <v>0.96910248307467006</v>
       </c>
       <c r="Q15" s="26">
         <f t="shared" si="7"/>
-        <v>1.378325874128159</v>
+        <v>0.98443002954738745</v>
       </c>
       <c r="R15" s="26">
         <f t="shared" si="7"/>
-        <v>1.7706869002943542</v>
+        <v>0.9032493609063843</v>
       </c>
       <c r="S15" s="26">
         <f t="shared" si="7"/>
-        <v>1.330671597462858</v>
+        <v>0.95039431864168056</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -46381,10 +46422,75 @@
       <c r="Q40" s="12"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
       <c r="Q41" s="12"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q42" s="12"/>
+      <c r="A42" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C42" s="1">
+        <v>64</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
+      <c r="E42" s="4">
+        <v>400</v>
+      </c>
+      <c r="F42" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G42" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H42" s="4">
+        <v>40</v>
+      </c>
+      <c r="I42" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J42" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K42" s="16">
+        <v>5000</v>
+      </c>
+      <c r="L42" s="14">
+        <v>1.3784722222222224E-2</v>
+      </c>
+      <c r="M42" s="8">
+        <v>5.5509875709120401E-2</v>
+      </c>
+      <c r="N42" s="25">
+        <f t="array" ref="N42">INDEX('Default Errors'!$J$7:$J$27,MATCH(C42&amp;D42,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.6252051388873606E-2</v>
+      </c>
+      <c r="O42" s="25">
+        <f t="array" ref="O42">INDEX('Default Errors'!$K$7:$K$27,MATCH(C42&amp;D42,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.7343418758699702E-2</v>
+      </c>
+      <c r="P42" s="9">
+        <f t="shared" ref="P42" si="12">M42/N42</f>
+        <v>0.83785897259692621</v>
+      </c>
+      <c r="Q42" s="9">
+        <f t="shared" ref="Q42" si="13">SQRT(P42)</f>
+        <v>0.91534636755543319</v>
+      </c>
+      <c r="R42" s="9">
+        <f t="shared" ref="R42" si="14">M42/O42</f>
+        <v>0.82428063101488158</v>
+      </c>
+      <c r="S42" s="9">
+        <f t="shared" ref="S42" si="15">SQRT(R42)</f>
+        <v>0.90789902027421621</v>
+      </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q43" s="12"/>
@@ -46393,105 +46499,1446 @@
       <c r="Q44" s="12"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="Q45" s="12"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q46" s="12"/>
+      <c r="A46" s="3">
+        <v>1</v>
+      </c>
+      <c r="B46" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C46" s="1">
+        <v>4</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
+      <c r="E46" s="4">
+        <v>400</v>
+      </c>
+      <c r="F46" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G46" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="H46" s="4">
+        <v>42</v>
+      </c>
+      <c r="I46" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J46" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="K46" s="16">
+        <v>5</v>
+      </c>
+      <c r="L46" s="14">
+        <v>5.7870370370370366E-5</v>
+      </c>
+      <c r="M46" s="22">
+        <v>2.5193958081904099E-4</v>
+      </c>
+      <c r="N46" s="25">
+        <f t="array" ref="N46">INDEX('Default Errors'!$J$7:$J$27,MATCH(C46&amp;D46,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>5.3403859472996501E-2</v>
+      </c>
+      <c r="O46" s="25">
+        <f t="array" ref="O46">INDEX('Default Errors'!$K$7:$K$27,MATCH(C46&amp;D46,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>1.35087180411301E-2</v>
+      </c>
+      <c r="P46" s="9">
+        <f>M46/N46</f>
+        <v>4.7176287127044343E-3</v>
+      </c>
+      <c r="Q46" s="9">
+        <f>SQRT(P46)</f>
+        <v>6.8684996270688067E-2</v>
+      </c>
+      <c r="R46" s="9">
+        <f>M46/O46</f>
+        <v>1.8650147264304324E-2</v>
+      </c>
+      <c r="S46" s="9">
+        <f>SQRT(R46)</f>
+        <v>0.13656554200933824</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>2</v>
+      </c>
+      <c r="B47" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C47" s="1">
+        <v>8</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="4">
+        <v>50</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G47" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="H47" s="4">
+        <v>42</v>
+      </c>
+      <c r="I47" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J47" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="K47" s="16">
+        <v>5</v>
+      </c>
+      <c r="L47" s="14">
+        <v>9.2592592592592588E-5</v>
+      </c>
+      <c r="M47" s="8">
+        <v>2.33682990516437E-3</v>
+      </c>
+      <c r="N47" s="25">
+        <f t="array" ref="N47">INDEX('Default Errors'!$J$7:$J$27,MATCH(C47&amp;D47,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.0828541567298902E-2</v>
+      </c>
+      <c r="O47" s="25">
+        <f t="array" ref="O47">INDEX('Default Errors'!$K$7:$K$27,MATCH(C47&amp;D47,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>3.0317906985562901E-2</v>
+      </c>
+      <c r="P47" s="9">
+        <f t="shared" ref="P47:P66" si="16">M47/N47</f>
+        <v>3.8416668309875064E-2</v>
+      </c>
+      <c r="Q47" s="9">
+        <f t="shared" ref="Q47:Q66" si="17">SQRT(P47)</f>
+        <v>0.19600170486471558</v>
+      </c>
+      <c r="R47" s="9">
+        <f t="shared" ref="R47:R66" si="18">M47/O47</f>
+        <v>7.7077547149846007E-2</v>
+      </c>
+      <c r="S47" s="9">
+        <f t="shared" ref="S47:S66" si="19">SQRT(R47)</f>
+        <v>0.27762843361198797</v>
+      </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q48" s="12"/>
-    </row>
-    <row r="49" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q49" s="12"/>
-    </row>
-    <row r="50" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q50" s="12"/>
-    </row>
-    <row r="51" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q51" s="12"/>
-    </row>
-    <row r="52" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q52" s="12"/>
-    </row>
-    <row r="53" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q53" s="12"/>
-    </row>
-    <row r="54" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q54" s="12"/>
-    </row>
-    <row r="55" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q55" s="12"/>
-    </row>
-    <row r="56" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q56" s="12"/>
-    </row>
-    <row r="57" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q57" s="12"/>
-    </row>
-    <row r="58" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q58" s="12"/>
-    </row>
-    <row r="59" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q59" s="12"/>
-    </row>
-    <row r="60" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q60" s="12"/>
-    </row>
-    <row r="61" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q61" s="12"/>
-    </row>
-    <row r="62" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q62" s="12"/>
-    </row>
-    <row r="63" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q63" s="12"/>
-    </row>
-    <row r="64" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q64" s="12"/>
-    </row>
-    <row r="65" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q65" s="12"/>
-    </row>
-    <row r="67" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>3</v>
+      </c>
+      <c r="B48" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C48" s="1">
+        <v>16</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="4">
+        <v>200</v>
+      </c>
+      <c r="F48" s="4">
+        <v>3</v>
+      </c>
+      <c r="G48" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="H48" s="4">
+        <v>42</v>
+      </c>
+      <c r="I48" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J48" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K48" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="L48" s="14">
+        <v>3.8194444444444446E-4</v>
+      </c>
+      <c r="M48" s="8">
+        <v>1.9997089525738702E-2</v>
+      </c>
+      <c r="N48" s="25">
+        <f t="array" ref="N48">INDEX('Default Errors'!$J$7:$J$27,MATCH(C48&amp;D48,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.6075900603069407E-2</v>
+      </c>
+      <c r="O48" s="25">
+        <f t="array" ref="O48">INDEX('Default Errors'!$K$7:$K$27,MATCH(C48&amp;D48,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>4.71924397561789E-2</v>
+      </c>
+      <c r="P48" s="9">
+        <f t="shared" si="16"/>
+        <v>0.30263816827658618</v>
+      </c>
+      <c r="Q48" s="9">
+        <f t="shared" si="17"/>
+        <v>0.55012559318448928</v>
+      </c>
+      <c r="R48" s="9">
+        <f t="shared" si="18"/>
+        <v>0.42373502258103718</v>
+      </c>
+      <c r="S48" s="9">
+        <f t="shared" si="19"/>
+        <v>0.65094932412672279</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>4</v>
+      </c>
+      <c r="B49" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C49" s="1">
+        <v>32</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" s="4">
+        <v>50</v>
+      </c>
+      <c r="F49" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="G49" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="H49" s="4">
+        <v>42</v>
+      </c>
+      <c r="I49" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J49" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K49" s="16">
+        <v>5000</v>
+      </c>
+      <c r="L49" s="14">
+        <v>1.0532407407407407E-3</v>
+      </c>
+      <c r="M49" s="8">
+        <v>4.23995426636763E-2</v>
+      </c>
+      <c r="N49" s="25">
+        <f t="array" ref="N49">INDEX('Default Errors'!$J$7:$J$27,MATCH(C49&amp;D49,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.4467693182005903E-2</v>
+      </c>
+      <c r="O49" s="25">
+        <f t="array" ref="O49">INDEX('Default Errors'!$K$7:$K$27,MATCH(C49&amp;D49,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.1261486472077201E-2</v>
+      </c>
+      <c r="P49" s="9">
+        <f t="shared" si="16"/>
+        <v>0.657686673291899</v>
+      </c>
+      <c r="Q49" s="9">
+        <f t="shared" si="17"/>
+        <v>0.81097883652528135</v>
+      </c>
+      <c r="R49" s="9">
+        <f t="shared" si="18"/>
+        <v>0.69210763736531078</v>
+      </c>
+      <c r="S49" s="9">
+        <f t="shared" si="19"/>
+        <v>0.83193006759301036</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>5</v>
+      </c>
+      <c r="B50" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C50" s="1">
+        <v>64</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="4">
+        <v>400</v>
+      </c>
+      <c r="F50" s="4">
+        <v>3</v>
+      </c>
+      <c r="G50" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H50" s="4">
+        <v>39</v>
+      </c>
+      <c r="I50" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J50" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="K50" s="16">
+        <v>5000</v>
+      </c>
+      <c r="L50" s="14">
+        <v>1.2604166666666666E-2</v>
+      </c>
+      <c r="M50" s="8">
+        <v>5.3888242223566203E-2</v>
+      </c>
+      <c r="N50" s="25">
+        <f t="array" ref="N50">INDEX('Default Errors'!$J$7:$J$27,MATCH(C50&amp;D50,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.6252051388873606E-2</v>
+      </c>
+      <c r="O50" s="25">
+        <f t="array" ref="O50">INDEX('Default Errors'!$K$7:$K$27,MATCH(C50&amp;D50,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.7343418758699702E-2</v>
+      </c>
+      <c r="P50" s="9">
+        <f t="shared" si="16"/>
+        <v>0.81338224392877012</v>
+      </c>
+      <c r="Q50" s="9">
+        <f t="shared" si="17"/>
+        <v>0.90187706697130854</v>
+      </c>
+      <c r="R50" s="9">
+        <f t="shared" si="18"/>
+        <v>0.80020057218441554</v>
+      </c>
+      <c r="S50" s="9">
+        <f t="shared" si="19"/>
+        <v>0.89453930723273167</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>6</v>
+      </c>
+      <c r="B51" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C51" s="1">
+        <v>128</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
+      <c r="E51" s="4">
+        <v>200</v>
+      </c>
+      <c r="F51" s="4">
+        <v>3</v>
+      </c>
+      <c r="G51" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H51" s="4">
+        <v>41</v>
+      </c>
+      <c r="I51" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J51" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K51" s="16">
+        <v>50000</v>
+      </c>
+      <c r="L51" s="14">
+        <v>3.8599537037037036E-2</v>
+      </c>
+      <c r="M51" s="8">
+        <v>6.5956359710807794E-2</v>
+      </c>
+      <c r="N51" s="25">
+        <f t="array" ref="N51">INDEX('Default Errors'!$J$7:$J$27,MATCH(C51&amp;D51,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.6204068387367407E-2</v>
+      </c>
+      <c r="O51" s="25">
+        <f t="array" ref="O51">INDEX('Default Errors'!$K$7:$K$27,MATCH(C51&amp;D51,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.67588650253087E-2</v>
+      </c>
+      <c r="P51" s="9">
+        <f t="shared" si="16"/>
+        <v>0.99625840703459123</v>
+      </c>
+      <c r="Q51" s="9">
+        <f t="shared" si="17"/>
+        <v>0.99812745029609884</v>
+      </c>
+      <c r="R51" s="9">
+        <f t="shared" si="18"/>
+        <v>0.98797904496733624</v>
+      </c>
+      <c r="S51" s="9">
+        <f t="shared" si="19"/>
+        <v>0.99397135017430771</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>7</v>
+      </c>
+      <c r="B52" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C52" s="1">
+        <v>4</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2</v>
+      </c>
+      <c r="E52" s="4">
+        <v>400</v>
+      </c>
+      <c r="F52" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G52" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="H52" s="4">
+        <v>42</v>
+      </c>
+      <c r="I52" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J52" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="K52" s="16">
+        <v>5</v>
+      </c>
+      <c r="L52" s="14">
+        <v>8.1018518518518516E-5</v>
+      </c>
+      <c r="M52" s="22">
+        <v>2.5193958081904099E-4</v>
+      </c>
+      <c r="N52" s="25">
+        <f t="array" ref="N52">INDEX('Default Errors'!$J$7:$J$27,MATCH(C52&amp;D52,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>5.3403859472996501E-2</v>
+      </c>
+      <c r="O52" s="25">
+        <f t="array" ref="O52">INDEX('Default Errors'!$K$7:$K$27,MATCH(C52&amp;D52,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>1.35087180411301E-2</v>
+      </c>
+      <c r="P52" s="9">
+        <f t="shared" si="16"/>
+        <v>4.7176287127044343E-3</v>
+      </c>
+      <c r="Q52" s="9">
+        <f t="shared" si="17"/>
+        <v>6.8684996270688067E-2</v>
+      </c>
+      <c r="R52" s="9">
+        <f t="shared" si="18"/>
+        <v>1.8650147264304324E-2</v>
+      </c>
+      <c r="S52" s="9">
+        <f t="shared" si="19"/>
+        <v>0.13656554200933824</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>8</v>
+      </c>
+      <c r="B53" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C53" s="1">
+        <v>8</v>
+      </c>
+      <c r="D53" s="1">
+        <v>2</v>
+      </c>
+      <c r="E53" s="4">
+        <v>50</v>
+      </c>
+      <c r="F53" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G53" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="H53" s="4">
+        <v>42</v>
+      </c>
+      <c r="I53" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J53" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="K53" s="16">
+        <v>5</v>
+      </c>
+      <c r="L53" s="14">
+        <v>1.1574074074074073E-4</v>
+      </c>
+      <c r="M53" s="8">
+        <v>2.3368299051645899E-3</v>
+      </c>
+      <c r="N53" s="25">
+        <f t="array" ref="N53">INDEX('Default Errors'!$J$7:$J$27,MATCH(C53&amp;D53,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.0828541567298902E-2</v>
+      </c>
+      <c r="O53" s="25">
+        <f t="array" ref="O53">INDEX('Default Errors'!$K$7:$K$27,MATCH(C53&amp;D53,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>3.0317906985562901E-2</v>
+      </c>
+      <c r="P53" s="9">
+        <f t="shared" si="16"/>
+        <v>3.8416668309878679E-2</v>
+      </c>
+      <c r="Q53" s="9">
+        <f t="shared" si="17"/>
+        <v>0.19600170486472479</v>
+      </c>
+      <c r="R53" s="9">
+        <f t="shared" si="18"/>
+        <v>7.7077547149853251E-2</v>
+      </c>
+      <c r="S53" s="9">
+        <f t="shared" si="19"/>
+        <v>0.27762843361200101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>9</v>
+      </c>
+      <c r="B54" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C54" s="1">
+        <v>16</v>
+      </c>
+      <c r="D54" s="1">
+        <v>2</v>
+      </c>
+      <c r="E54" s="4">
+        <v>200</v>
+      </c>
+      <c r="F54" s="4">
+        <v>3</v>
+      </c>
+      <c r="G54" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H54" s="4">
+        <v>42</v>
+      </c>
+      <c r="I54" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J54" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K54" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="L54" s="14">
+        <v>3.9351851851851852E-4</v>
+      </c>
+      <c r="M54" s="8">
+        <v>1.88640143419549E-2</v>
+      </c>
+      <c r="N54" s="25">
+        <f t="array" ref="N54">INDEX('Default Errors'!$J$7:$J$27,MATCH(C54&amp;D54,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.6075900603069407E-2</v>
+      </c>
+      <c r="O54" s="25">
+        <f t="array" ref="O54">INDEX('Default Errors'!$K$7:$K$27,MATCH(C54&amp;D54,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>4.71924397561789E-2</v>
+      </c>
+      <c r="P54" s="9">
+        <f t="shared" si="16"/>
+        <v>0.28549008291653333</v>
+      </c>
+      <c r="Q54" s="9">
+        <f t="shared" si="17"/>
+        <v>0.53431272015228437</v>
+      </c>
+      <c r="R54" s="9">
+        <f t="shared" si="18"/>
+        <v>0.39972534667451765</v>
+      </c>
+      <c r="S54" s="9">
+        <f t="shared" si="19"/>
+        <v>0.63223836222940288</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>10</v>
+      </c>
+      <c r="B55" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C55" s="1">
+        <v>32</v>
+      </c>
+      <c r="D55" s="1">
+        <v>2</v>
+      </c>
+      <c r="E55" s="4">
+        <v>50</v>
+      </c>
+      <c r="F55" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="G55" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="H55" s="4">
+        <v>42</v>
+      </c>
+      <c r="I55" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J55" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K55" s="16">
+        <v>50000</v>
+      </c>
+      <c r="L55" s="14">
+        <v>1.0300925925925926E-3</v>
+      </c>
+      <c r="M55" s="8">
+        <v>5.2774327512604399E-2</v>
+      </c>
+      <c r="N55" s="25">
+        <f t="array" ref="N55">INDEX('Default Errors'!$J$7:$J$27,MATCH(C55&amp;D55,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.4467693182005903E-2</v>
+      </c>
+      <c r="O55" s="25">
+        <f t="array" ref="O55">INDEX('Default Errors'!$K$7:$K$27,MATCH(C55&amp;D55,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.1261486472077201E-2</v>
+      </c>
+      <c r="P55" s="9">
+        <f t="shared" si="16"/>
+        <v>0.81861665754987289</v>
+      </c>
+      <c r="Q55" s="9">
+        <f t="shared" si="17"/>
+        <v>0.90477436830950997</v>
+      </c>
+      <c r="R55" s="9">
+        <f t="shared" si="18"/>
+        <v>0.86146012040792996</v>
+      </c>
+      <c r="S55" s="9">
+        <f t="shared" si="19"/>
+        <v>0.92814875984829603</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>11</v>
+      </c>
+      <c r="B56" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C56" s="1">
+        <v>64</v>
+      </c>
+      <c r="D56" s="1">
+        <v>2</v>
+      </c>
+      <c r="E56" s="4">
+        <v>400</v>
+      </c>
+      <c r="F56" s="4">
+        <v>3</v>
+      </c>
+      <c r="G56" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H56" s="4">
+        <v>39</v>
+      </c>
+      <c r="I56" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J56" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="K56" s="16">
+        <v>5000</v>
+      </c>
+      <c r="L56" s="14">
+        <v>1.3657407407407408E-2</v>
+      </c>
+      <c r="M56" s="8">
+        <v>5.3888242223566203E-2</v>
+      </c>
+      <c r="N56" s="25">
+        <f t="array" ref="N56">INDEX('Default Errors'!$J$7:$J$27,MATCH(C56&amp;D56,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.6252051388873606E-2</v>
+      </c>
+      <c r="O56" s="25">
+        <f t="array" ref="O56">INDEX('Default Errors'!$K$7:$K$27,MATCH(C56&amp;D56,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.7343418758699702E-2</v>
+      </c>
+      <c r="P56" s="9">
+        <f t="shared" si="16"/>
+        <v>0.81338224392877012</v>
+      </c>
+      <c r="Q56" s="9">
+        <f t="shared" si="17"/>
+        <v>0.90187706697130854</v>
+      </c>
+      <c r="R56" s="9">
+        <f t="shared" si="18"/>
+        <v>0.80020057218441554</v>
+      </c>
+      <c r="S56" s="9">
+        <f t="shared" si="19"/>
+        <v>0.89453930723273167</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>12</v>
+      </c>
+      <c r="B57" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C57" s="1">
+        <v>128</v>
+      </c>
+      <c r="D57" s="1">
+        <v>2</v>
+      </c>
+      <c r="E57" s="4">
+        <v>200</v>
+      </c>
+      <c r="F57" s="4">
+        <v>3</v>
+      </c>
+      <c r="G57" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H57" s="4">
+        <v>41</v>
+      </c>
+      <c r="I57" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J57" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K57" s="16">
+        <v>50000</v>
+      </c>
+      <c r="L57" s="14">
+        <v>3.7696759259259256E-2</v>
+      </c>
+      <c r="M57" s="8">
+        <v>6.5956359710807794E-2</v>
+      </c>
+      <c r="N57" s="25">
+        <f t="array" ref="N57">INDEX('Default Errors'!$J$7:$J$27,MATCH(C57&amp;D57,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.6204068387367407E-2</v>
+      </c>
+      <c r="O57" s="25">
+        <f t="array" ref="O57">INDEX('Default Errors'!$K$7:$K$27,MATCH(C57&amp;D57,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.67588650253087E-2</v>
+      </c>
+      <c r="P57" s="9">
+        <f t="shared" si="16"/>
+        <v>0.99625840703459123</v>
+      </c>
+      <c r="Q57" s="9">
+        <f t="shared" si="17"/>
+        <v>0.99812745029609884</v>
+      </c>
+      <c r="R57" s="9">
+        <f t="shared" si="18"/>
+        <v>0.98797904496733624</v>
+      </c>
+      <c r="S57" s="9">
+        <f t="shared" si="19"/>
+        <v>0.99397135017430771</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>13</v>
+      </c>
+      <c r="B58" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C58" s="1">
+        <v>4</v>
+      </c>
+      <c r="D58" s="1">
+        <v>3</v>
+      </c>
+      <c r="E58" s="4">
+        <v>400</v>
+      </c>
+      <c r="F58" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G58" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="H58" s="4">
+        <v>42</v>
+      </c>
+      <c r="I58" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J58" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="K58" s="16">
+        <v>5</v>
+      </c>
+      <c r="L58" s="14">
+        <v>9.2592592592592588E-5</v>
+      </c>
+      <c r="M58" s="22">
+        <v>2.5193958081904099E-4</v>
+      </c>
+      <c r="N58" s="25">
+        <f t="array" ref="N58">INDEX('Default Errors'!$J$7:$J$27,MATCH(C58&amp;D58,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>5.3403859472996501E-2</v>
+      </c>
+      <c r="O58" s="25">
+        <f t="array" ref="O58">INDEX('Default Errors'!$K$7:$K$27,MATCH(C58&amp;D58,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>1.35087180411301E-2</v>
+      </c>
+      <c r="P58" s="9">
+        <f t="shared" si="16"/>
+        <v>4.7176287127044343E-3</v>
+      </c>
+      <c r="Q58" s="9">
+        <f t="shared" si="17"/>
+        <v>6.8684996270688067E-2</v>
+      </c>
+      <c r="R58" s="9">
+        <f t="shared" si="18"/>
+        <v>1.8650147264304324E-2</v>
+      </c>
+      <c r="S58" s="9">
+        <f t="shared" si="19"/>
+        <v>0.13656554200933824</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>14</v>
+      </c>
+      <c r="B59" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C59" s="1">
+        <v>8</v>
+      </c>
+      <c r="D59" s="1">
+        <v>3</v>
+      </c>
+      <c r="E59" s="4">
+        <v>50</v>
+      </c>
+      <c r="F59" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G59" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="H59" s="4">
+        <v>42</v>
+      </c>
+      <c r="I59" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J59" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="K59" s="16">
+        <v>5</v>
+      </c>
+      <c r="L59" s="14">
+        <v>9.2592592592592588E-5</v>
+      </c>
+      <c r="M59" s="8">
+        <v>2.33682990516437E-3</v>
+      </c>
+      <c r="N59" s="25">
+        <f t="array" ref="N59">INDEX('Default Errors'!$J$7:$J$27,MATCH(C59&amp;D59,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.0828541567298902E-2</v>
+      </c>
+      <c r="O59" s="25">
+        <f t="array" ref="O59">INDEX('Default Errors'!$K$7:$K$27,MATCH(C59&amp;D59,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>3.0317906985562901E-2</v>
+      </c>
+      <c r="P59" s="9">
+        <f t="shared" si="16"/>
+        <v>3.8416668309875064E-2</v>
+      </c>
+      <c r="Q59" s="9">
+        <f t="shared" si="17"/>
+        <v>0.19600170486471558</v>
+      </c>
+      <c r="R59" s="9">
+        <f t="shared" si="18"/>
+        <v>7.7077547149846007E-2</v>
+      </c>
+      <c r="S59" s="9">
+        <f t="shared" si="19"/>
+        <v>0.27762843361198797</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>15</v>
+      </c>
+      <c r="B60" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C60" s="1">
+        <v>16</v>
+      </c>
+      <c r="D60" s="1">
+        <v>3</v>
+      </c>
+      <c r="E60" s="4">
+        <v>200</v>
+      </c>
+      <c r="F60" s="4">
+        <v>3</v>
+      </c>
+      <c r="G60" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H60" s="4">
+        <v>42</v>
+      </c>
+      <c r="I60" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J60" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K60" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="L60" s="14">
+        <v>3.9351851851851852E-4</v>
+      </c>
+      <c r="M60" s="8">
+        <v>1.88640143419549E-2</v>
+      </c>
+      <c r="N60" s="25">
+        <f t="array" ref="N60">INDEX('Default Errors'!$J$7:$J$27,MATCH(C60&amp;D60,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.6075900603069407E-2</v>
+      </c>
+      <c r="O60" s="25">
+        <f t="array" ref="O60">INDEX('Default Errors'!$K$7:$K$27,MATCH(C60&amp;D60,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>4.71924397561789E-2</v>
+      </c>
+      <c r="P60" s="9">
+        <f t="shared" si="16"/>
+        <v>0.28549008291653333</v>
+      </c>
+      <c r="Q60" s="9">
+        <f t="shared" si="17"/>
+        <v>0.53431272015228437</v>
+      </c>
+      <c r="R60" s="9">
+        <f t="shared" si="18"/>
+        <v>0.39972534667451765</v>
+      </c>
+      <c r="S60" s="9">
+        <f t="shared" si="19"/>
+        <v>0.63223836222940288</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>16</v>
+      </c>
+      <c r="B61" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C61" s="1">
+        <v>32</v>
+      </c>
+      <c r="D61" s="1">
+        <v>3</v>
+      </c>
+      <c r="E61" s="4">
+        <v>50</v>
+      </c>
+      <c r="F61" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="G61" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="H61" s="4">
+        <v>42</v>
+      </c>
+      <c r="I61" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J61" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K61" s="16">
+        <v>50000</v>
+      </c>
+      <c r="L61" s="14">
+        <v>1.0300925925925926E-3</v>
+      </c>
+      <c r="M61" s="8">
+        <v>5.2774327512604399E-2</v>
+      </c>
+      <c r="N61" s="25">
+        <f t="array" ref="N61">INDEX('Default Errors'!$J$7:$J$27,MATCH(C61&amp;D61,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.4467693182005903E-2</v>
+      </c>
+      <c r="O61" s="25">
+        <f t="array" ref="O61">INDEX('Default Errors'!$K$7:$K$27,MATCH(C61&amp;D61,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.1261486472077201E-2</v>
+      </c>
+      <c r="P61" s="9">
+        <f t="shared" si="16"/>
+        <v>0.81861665754987289</v>
+      </c>
+      <c r="Q61" s="9">
+        <f t="shared" si="17"/>
+        <v>0.90477436830950997</v>
+      </c>
+      <c r="R61" s="9">
+        <f t="shared" si="18"/>
+        <v>0.86146012040792996</v>
+      </c>
+      <c r="S61" s="9">
+        <f t="shared" si="19"/>
+        <v>0.92814875984829603</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>17</v>
+      </c>
+      <c r="B62" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C62" s="1">
+        <v>64</v>
+      </c>
+      <c r="D62" s="1">
+        <v>3</v>
+      </c>
+      <c r="E62" s="4">
+        <v>400</v>
+      </c>
+      <c r="F62" s="4">
+        <v>3</v>
+      </c>
+      <c r="G62" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H62" s="4">
+        <v>39</v>
+      </c>
+      <c r="I62" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J62" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="K62" s="16">
+        <v>5000</v>
+      </c>
+      <c r="L62" s="14">
+        <v>1.3819444444444445E-2</v>
+      </c>
+      <c r="M62" s="8">
+        <v>5.3888242223566203E-2</v>
+      </c>
+      <c r="N62" s="25">
+        <f t="array" ref="N62">INDEX('Default Errors'!$J$7:$J$27,MATCH(C62&amp;D62,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.6252051388873606E-2</v>
+      </c>
+      <c r="O62" s="25">
+        <f t="array" ref="O62">INDEX('Default Errors'!$K$7:$K$27,MATCH(C62&amp;D62,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.7343418758699702E-2</v>
+      </c>
+      <c r="P62" s="9">
+        <f t="shared" si="16"/>
+        <v>0.81338224392877012</v>
+      </c>
+      <c r="Q62" s="9">
+        <f t="shared" si="17"/>
+        <v>0.90187706697130854</v>
+      </c>
+      <c r="R62" s="9">
+        <f t="shared" si="18"/>
+        <v>0.80020057218441554</v>
+      </c>
+      <c r="S62" s="9">
+        <f t="shared" si="19"/>
+        <v>0.89453930723273167</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>18</v>
+      </c>
+      <c r="B63" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C63" s="1">
+        <v>128</v>
+      </c>
+      <c r="D63" s="1">
+        <v>3</v>
+      </c>
+      <c r="E63" s="4">
+        <v>200</v>
+      </c>
+      <c r="F63" s="4">
+        <v>3</v>
+      </c>
+      <c r="G63" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H63" s="4">
+        <v>41</v>
+      </c>
+      <c r="I63" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J63" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K63" s="16">
+        <v>50000</v>
+      </c>
+      <c r="L63" s="14">
+        <v>3.8865740740740742E-2</v>
+      </c>
+      <c r="M63" s="8">
+        <v>6.5956359710807794E-2</v>
+      </c>
+      <c r="N63" s="25">
+        <f t="array" ref="N63">INDEX('Default Errors'!$J$7:$J$27,MATCH(C63&amp;D63,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.6204068387367407E-2</v>
+      </c>
+      <c r="O63" s="25">
+        <f t="array" ref="O63">INDEX('Default Errors'!$K$7:$K$27,MATCH(C63&amp;D63,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.67588650253087E-2</v>
+      </c>
+      <c r="P63" s="9">
+        <f t="shared" si="16"/>
+        <v>0.99625840703459123</v>
+      </c>
+      <c r="Q63" s="9">
+        <f t="shared" si="17"/>
+        <v>0.99812745029609884</v>
+      </c>
+      <c r="R63" s="9">
+        <f t="shared" si="18"/>
+        <v>0.98797904496733624</v>
+      </c>
+      <c r="S63" s="9">
+        <f t="shared" si="19"/>
+        <v>0.99397135017430771</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <v>19</v>
+      </c>
+      <c r="B64" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C64" s="1">
+        <v>146</v>
+      </c>
+      <c r="D64" s="1">
+        <v>1</v>
+      </c>
+      <c r="E64" s="4">
+        <v>200</v>
+      </c>
+      <c r="F64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G64" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H64" s="4">
+        <v>39</v>
+      </c>
+      <c r="I64" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J64" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="K64" s="16">
+        <v>50000</v>
+      </c>
+      <c r="L64" s="14">
+        <v>5.3275462962962962E-2</v>
+      </c>
+      <c r="M64" s="8">
+        <v>6.5437954795161096E-2</v>
+      </c>
+      <c r="N64" s="25">
+        <f t="array" ref="N64">INDEX('Default Errors'!$J$7:$J$27,MATCH(C64&amp;D64,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.6727707642842707E-2</v>
+      </c>
+      <c r="O64" s="25">
+        <f t="array" ref="O64">INDEX('Default Errors'!$K$7:$K$27,MATCH(C64&amp;D64,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>7.1774028116071004E-2</v>
+      </c>
+      <c r="P64" s="9">
+        <f t="shared" si="16"/>
+        <v>0.98067140482953563</v>
+      </c>
+      <c r="Q64" s="9">
+        <f t="shared" si="17"/>
+        <v>0.99028854624777707</v>
+      </c>
+      <c r="R64" s="9">
+        <f t="shared" si="18"/>
+        <v>0.91172192104554339</v>
+      </c>
+      <c r="S64" s="9">
+        <f t="shared" si="19"/>
+        <v>0.95484130673402656</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
+        <v>20</v>
+      </c>
+      <c r="B65" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C65" s="1">
+        <v>146</v>
+      </c>
+      <c r="D65" s="1">
+        <v>2</v>
+      </c>
+      <c r="E65" s="4">
+        <v>200</v>
+      </c>
+      <c r="F65" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G65" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H65" s="4">
+        <v>39</v>
+      </c>
+      <c r="I65" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J65" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="K65" s="16">
+        <v>50000</v>
+      </c>
+      <c r="L65" s="14">
+        <v>5.3321759259259256E-2</v>
+      </c>
+      <c r="M65" s="8">
+        <v>6.5437954795161096E-2</v>
+      </c>
+      <c r="N65" s="25">
+        <f t="array" ref="N65">INDEX('Default Errors'!$J$7:$J$27,MATCH(C65&amp;D65,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.6727707642842707E-2</v>
+      </c>
+      <c r="O65" s="25">
+        <f t="array" ref="O65">INDEX('Default Errors'!$K$7:$K$27,MATCH(C65&amp;D65,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>7.1774028116071004E-2</v>
+      </c>
+      <c r="P65" s="9">
+        <f t="shared" si="16"/>
+        <v>0.98067140482953563</v>
+      </c>
+      <c r="Q65" s="9">
+        <f t="shared" si="17"/>
+        <v>0.99028854624777707</v>
+      </c>
+      <c r="R65" s="9">
+        <f t="shared" si="18"/>
+        <v>0.91172192104554339</v>
+      </c>
+      <c r="S65" s="9">
+        <f t="shared" si="19"/>
+        <v>0.95484130673402656</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
+        <v>21</v>
+      </c>
+      <c r="B66" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C66" s="1">
+        <v>148</v>
+      </c>
+      <c r="D66" s="1">
+        <v>1</v>
+      </c>
+      <c r="E66" s="4">
+        <v>200</v>
+      </c>
+      <c r="F66" s="4">
+        <v>3</v>
+      </c>
+      <c r="G66" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H66" s="4">
+        <v>40</v>
+      </c>
+      <c r="I66" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J66" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K66" s="16">
+        <v>50000</v>
+      </c>
+      <c r="L66" s="14">
+        <v>5.4479166666666669E-2</v>
+      </c>
+      <c r="M66" s="8">
+        <v>6.4880812799093399E-2</v>
+      </c>
+      <c r="N66" s="25">
+        <f t="array" ref="N66">INDEX('Default Errors'!$J$7:$J$27,MATCH(C66&amp;D66,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>6.6949382477326999E-2</v>
+      </c>
+      <c r="O66" s="25">
+        <f t="array" ref="O66">INDEX('Default Errors'!$K$7:$K$27,MATCH(C66&amp;D66,'Default Errors'!$H$7:$H$27&amp;'Default Errors'!$I$7:$I$27,0))</f>
+        <v>7.1830455251014405E-2</v>
+      </c>
+      <c r="P66" s="9">
+        <f t="shared" si="16"/>
+        <v>0.96910248307467006</v>
+      </c>
+      <c r="Q66" s="9">
+        <f t="shared" si="17"/>
+        <v>0.98443002954738745</v>
+      </c>
+      <c r="R66" s="9">
+        <f t="shared" si="18"/>
+        <v>0.9032493609063843</v>
+      </c>
+      <c r="S66" s="9">
+        <f t="shared" si="19"/>
+        <v>0.95039431864168056</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q67" s="12"/>
     </row>
-    <row r="68" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q68" s="12"/>
     </row>
-    <row r="69" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q69" s="12"/>
     </row>
-    <row r="70" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q70" s="12"/>
     </row>
-    <row r="71" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q71" s="12"/>
     </row>
-    <row r="72" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q72" s="12"/>
     </row>
-    <row r="73" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q73" s="12"/>
     </row>
-    <row r="74" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q74" s="12"/>
     </row>
-    <row r="75" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q75" s="12"/>
     </row>
-    <row r="76" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q76" s="12"/>
     </row>
-    <row r="77" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q77" s="12"/>
     </row>
-    <row r="78" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q78" s="12"/>
     </row>
-    <row r="79" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q79" s="12"/>
     </row>
-    <row r="80" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q80" s="12"/>
     </row>
     <row r="81" spans="17:17" x14ac:dyDescent="0.25">
@@ -46519,8 +47966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:U84"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46586,15 +48033,15 @@
       </c>
       <c r="F8" s="7">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="G8" s="7">
         <f t="shared" si="0"/>
-        <v>0.95</v>
+        <v>0.7</v>
       </c>
       <c r="H8" s="7">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I8" s="7">
         <f t="shared" si="0"/>
@@ -46602,37 +48049,37 @@
       </c>
       <c r="J8" s="7">
         <f t="shared" si="0"/>
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K8" s="7">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="L8" s="20">
         <f t="shared" si="0"/>
-        <v>3.4722222222222222E-5</v>
+        <v>5.7870370370370366E-5</v>
       </c>
       <c r="M8" s="7">
         <f t="shared" si="0"/>
-        <v>7.0206791531473407E-5</v>
+        <v>4.7599406016720803E-5</v>
       </c>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="26">
         <f>INDEX(P$17:P$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,4),$M$17:$M$999,))</f>
-        <v>4.7171127603667316E-4</v>
+        <v>3.1981487917261402E-4</v>
       </c>
       <c r="Q8" s="26">
         <f>INDEX(Q$17:Q$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,4),$M$17:$M$999,))</f>
-        <v>2.1718915167122717E-2</v>
+        <v>1.7883368787021476E-2</v>
       </c>
       <c r="R8" s="26">
         <f>INDEX(R$17:R$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,4),$M$17:$M$999,))</f>
-        <v>3.7621417592975989E-3</v>
+        <v>2.5506893163318514E-3</v>
       </c>
       <c r="S8" s="26">
         <f>INDEX(S$17:S$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,4),$M$17:$M$999,))</f>
-        <v>6.1336300502211567E-2</v>
+        <v>5.0504349479345352E-2</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
@@ -46646,7 +48093,7 @@
       </c>
       <c r="D9" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" si="1"/>
@@ -46654,15 +48101,15 @@
       </c>
       <c r="F9" s="7">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="G9" s="7">
         <f t="shared" si="1"/>
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="H9" s="7">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="1"/>
@@ -46674,33 +48121,33 @@
       </c>
       <c r="K9" s="7">
         <f t="shared" si="1"/>
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="L9" s="20">
         <f t="shared" si="1"/>
-        <v>1.6203703703703703E-4</v>
+        <v>1.7361111111111112E-4</v>
       </c>
       <c r="M9" s="7">
         <f t="shared" si="1"/>
-        <v>2.5342259253738099E-3</v>
+        <v>1.9960414350355298E-3</v>
       </c>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="26">
         <f>INDEX(P$17:P$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,8),$M$17:$M$999,))</f>
-        <v>1.6958074431713391E-2</v>
+        <v>1.3356748853843263E-2</v>
       </c>
       <c r="Q9" s="26">
         <f>INDEX(Q$17:Q$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,8),$M$17:$M$999,))</f>
-        <v>0.13022317163897287</v>
+        <v>0.11557140153966838</v>
       </c>
       <c r="R9" s="26">
         <f>INDEX(R$17:R$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,8),$M$17:$M$999,))</f>
-        <v>4.3579339636089919E-2</v>
+        <v>3.4324551238378957E-2</v>
       </c>
       <c r="S9" s="26">
         <f>INDEX(S$17:S$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,8),$M$17:$M$999,))</f>
-        <v>0.20875665171699301</v>
+        <v>0.18526886203131643</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
@@ -46722,11 +48169,11 @@
       </c>
       <c r="F10" s="7">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="G10" s="7">
         <f t="shared" si="2"/>
-        <v>0.9</v>
+        <v>0.2</v>
       </c>
       <c r="H10" s="7">
         <f t="shared" si="2"/>
@@ -46734,41 +48181,41 @@
       </c>
       <c r="I10" s="7">
         <f t="shared" si="2"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J10" s="7">
         <f t="shared" si="2"/>
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K10" s="7">
         <f t="shared" si="2"/>
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="L10" s="20">
         <f t="shared" si="2"/>
-        <v>2.4305555555555552E-4</v>
+        <v>2.3148148148148146E-4</v>
       </c>
       <c r="M10" s="7">
         <f t="shared" si="2"/>
-        <v>4.5017629759382602E-2</v>
+        <v>3.4603751124252097E-2</v>
       </c>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
       <c r="P10" s="26">
         <f>INDEX(P$17:P$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,16),$M$17:$M$999,))</f>
-        <v>0.30314983960036485</v>
+        <v>0.23302252159781048</v>
       </c>
       <c r="Q10" s="26">
         <f>INDEX(Q$17:Q$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,16),$M$17:$M$999,))</f>
-        <v>0.5505904463395318</v>
+        <v>0.48272406362000486</v>
       </c>
       <c r="R10" s="26">
         <f>INDEX(R$17:R$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,16),$M$17:$M$999,))</f>
-        <v>0.37862107644917764</v>
+        <v>0.29103508047562415</v>
       </c>
       <c r="S10" s="26">
         <f>INDEX(S$17:S$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,16),$M$17:$M$999,))</f>
-        <v>0.61532192911449013</v>
+        <v>0.53947667278170996</v>
       </c>
       <c r="U10" s="15"/>
     </row>
@@ -46787,11 +48234,11 @@
       </c>
       <c r="E11" s="7">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>1.5</v>
       </c>
       <c r="G11" s="7">
         <f t="shared" si="3"/>
@@ -46799,45 +48246,45 @@
       </c>
       <c r="H11" s="7">
         <f t="shared" si="3"/>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="J11" s="7">
         <f t="shared" si="3"/>
-        <v>1.0000000000000001E-5</v>
+        <v>1E-4</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" si="3"/>
-        <v>0.05</v>
+        <v>5000</v>
       </c>
       <c r="L11" s="20">
         <f t="shared" si="3"/>
-        <v>9.9537037037037042E-4</v>
+        <v>1.5162037037037036E-3</v>
       </c>
       <c r="M11" s="7">
         <f t="shared" si="3"/>
-        <v>9.1706502332364895E-2</v>
+        <v>8.5608063744124802E-2</v>
       </c>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="26">
         <f>INDEX(P$17:P$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,32),$M$17:$M$999,))</f>
-        <v>0.63032060754071295</v>
+        <v>0.58840458830297326</v>
       </c>
       <c r="Q11" s="26">
         <f>INDEX(Q$17:Q$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,32),$M$17:$M$999,))</f>
-        <v>0.79392733139797689</v>
+        <v>0.76707534721367054</v>
       </c>
       <c r="R11" s="26">
         <f>INDEX(R$17:R$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,32),$M$17:$M$999,))</f>
-        <v>0.64764761071847277</v>
+        <v>0.60457935404815888</v>
       </c>
       <c r="S11" s="26">
         <f>INDEX(S$17:S$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,32),$M$17:$M$999,))</f>
-        <v>0.80476556258234155</v>
+        <v>0.7775470108283864</v>
       </c>
       <c r="U11" s="15"/>
     </row>
@@ -46852,23 +48299,23 @@
       </c>
       <c r="D12" s="7">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E12" s="7">
         <f t="shared" si="4"/>
-        <v>50</v>
+        <v>400</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="G12" s="7">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="H12" s="7">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I12" s="7">
         <f t="shared" si="4"/>
@@ -46880,33 +48327,33 @@
       </c>
       <c r="K12" s="7">
         <f t="shared" si="4"/>
-        <v>0.05</v>
+        <v>50000</v>
       </c>
       <c r="L12" s="20">
         <f t="shared" si="4"/>
-        <v>4.4907407407407405E-3</v>
+        <v>1.3958333333333335E-2</v>
       </c>
       <c r="M12" s="7">
         <f t="shared" si="4"/>
-        <v>0.146226345122142</v>
+        <v>0.129747710464202</v>
       </c>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
       <c r="P12" s="26">
         <f>INDEX(P$17:P$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,64),$M$17:$M$999,))</f>
-        <v>1.0110686894883125</v>
+        <v>0.89712867728159829</v>
       </c>
       <c r="Q12" s="26">
         <f>INDEX(Q$17:Q$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,64),$M$17:$M$999,))</f>
-        <v>1.005519114432099</v>
+        <v>0.94716876916503023</v>
       </c>
       <c r="R12" s="26">
         <f>INDEX(R$17:R$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,64),$M$17:$M$999,))</f>
-        <v>0.99895610186040507</v>
+        <v>0.88638108927886672</v>
       </c>
       <c r="S12" s="26">
         <f>INDEX(S$17:S$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,64),$M$17:$M$999,))</f>
-        <v>0.99947791464364288</v>
+        <v>0.94147814062720903</v>
       </c>
       <c r="U12" s="15"/>
     </row>
@@ -46929,15 +48376,15 @@
       </c>
       <c r="F13" s="7">
         <f t="shared" si="5"/>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="G13" s="7">
         <f t="shared" si="5"/>
-        <v>0.95</v>
+        <v>0.2</v>
       </c>
       <c r="H13" s="7">
         <f t="shared" si="5"/>
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I13" s="7">
         <f t="shared" si="5"/>
@@ -46949,7 +48396,7 @@
       </c>
       <c r="K13" s="7">
         <f t="shared" si="5"/>
-        <v>0.05</v>
+        <v>5000</v>
       </c>
       <c r="L13" s="20">
         <f t="shared" si="5"/>
@@ -46957,25 +48404,25 @@
       </c>
       <c r="M13" s="7">
         <f t="shared" si="5"/>
-        <v>0.20630408837236</v>
+        <v>0.15391466481192201</v>
       </c>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
       <c r="P13" s="26">
         <f>INDEX(P$17:P$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,128),$M$17:$M$999,))</f>
-        <v>1.4081473670903568</v>
+        <v>1.0505585794321088</v>
       </c>
       <c r="Q13" s="26">
         <f>INDEX(Q$17:Q$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,128),$M$17:$M$999,))</f>
-        <v>1.1866538531055957</v>
+        <v>1.0249675992108769</v>
       </c>
       <c r="R13" s="26">
         <f>INDEX(R$17:R$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,128),$M$17:$M$999,))</f>
-        <v>1.4016652206223299</v>
+        <v>1.0457225269391142</v>
       </c>
       <c r="S13" s="26">
         <f>INDEX(S$17:S$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,128),$M$17:$M$999,))</f>
-        <v>1.1839194316431882</v>
+        <v>1.0226057534255879</v>
       </c>
       <c r="U13" s="15"/>
     </row>
@@ -46998,7 +48445,7 @@
       </c>
       <c r="F14" s="7">
         <f t="shared" si="6"/>
-        <v>0.1</v>
+        <v>3</v>
       </c>
       <c r="G14" s="7">
         <f t="shared" si="6"/>
@@ -47006,45 +48453,45 @@
       </c>
       <c r="H14" s="7">
         <f t="shared" si="6"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I14" s="7">
         <f t="shared" si="6"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="J14" s="7">
         <f t="shared" si="6"/>
-        <v>1.0000000000000001E-5</v>
+        <v>1E-4</v>
       </c>
       <c r="K14" s="7">
         <f t="shared" si="6"/>
-        <v>0.05</v>
+        <v>500</v>
       </c>
       <c r="L14" s="20">
         <f t="shared" si="6"/>
-        <v>3.3379629629629634E-2</v>
+        <v>3.3599537037037039E-2</v>
       </c>
       <c r="M14" s="7">
         <f t="shared" si="6"/>
-        <v>0.18687459017129199</v>
+        <v>0.17220235429966699</v>
       </c>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="26">
         <f>INDEX(P$17:P$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,146),$M$17:$M$999,))</f>
-        <v>1.2676972436774152</v>
+        <v>1.1681655044720212</v>
       </c>
       <c r="Q14" s="26">
         <f>INDEX(Q$17:Q$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,146),$M$17:$M$999,))</f>
-        <v>1.1259206205045786</v>
+        <v>1.0808170541178657</v>
       </c>
       <c r="R14" s="26">
         <f>INDEX(R$17:R$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,146),$M$17:$M$999,))</f>
-        <v>1.1886057855234284</v>
+        <v>1.0952838179536666</v>
       </c>
       <c r="S14" s="26">
         <f>INDEX(S$17:S$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,146),$M$17:$M$999,))</f>
-        <v>1.090231987020849</v>
+        <v>1.0465580815003372</v>
       </c>
       <c r="U14" s="15"/>
     </row>
@@ -48566,75 +50013,1457 @@
       <c r="U39" s="12"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R40" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="S40" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="U40" s="12"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>1</v>
+      </c>
+      <c r="B41" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C41" s="1">
+        <v>4</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="4">
+        <v>400</v>
+      </c>
+      <c r="F41" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="G41" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="H41" s="4">
+        <v>41</v>
+      </c>
+      <c r="I41" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J41" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K41" s="16">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L41" s="14">
+        <v>5.7870370370370366E-5</v>
+      </c>
+      <c r="M41" s="22">
+        <v>4.7599406016720803E-5</v>
+      </c>
+      <c r="N41" s="25">
+        <f t="array" ref="N41">INDEX('Default Errors'!$E$7:$E$27,MATCH(C41&amp;D41,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.148834244797691</v>
+      </c>
+      <c r="O41" s="25">
+        <f t="array" ref="O41">INDEX('Default Errors'!$F$7:$F$27,MATCH(C41&amp;D41,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>1.8661389182894901E-2</v>
+      </c>
+      <c r="P41" s="9">
+        <f>M41/N41</f>
+        <v>3.1981487917261402E-4</v>
+      </c>
+      <c r="Q41" s="9">
+        <f>SQRT(P41)</f>
+        <v>1.7883368787021476E-2</v>
+      </c>
+      <c r="R41" s="9">
+        <f>M41/O41</f>
+        <v>2.5506893163318514E-3</v>
+      </c>
+      <c r="S41" s="9">
+        <f>SQRT(R41)</f>
+        <v>5.0504349479345352E-2</v>
+      </c>
       <c r="U41" s="12"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>2</v>
+      </c>
+      <c r="B42" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C42" s="1">
+        <v>8</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
+      <c r="E42" s="4">
+        <v>400</v>
+      </c>
+      <c r="F42" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G42" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H42" s="4">
+        <v>41</v>
+      </c>
+      <c r="I42" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J42" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K42" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="L42" s="14">
+        <v>1.5046296296296297E-4</v>
+      </c>
+      <c r="M42" s="8">
+        <v>1.99604143503802E-3</v>
+      </c>
+      <c r="N42" s="25">
+        <f t="array" ref="N42">INDEX('Default Errors'!$E$7:$E$27,MATCH(C42&amp;D42,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.14944066530540401</v>
+      </c>
+      <c r="O42" s="25">
+        <f t="array" ref="O42">INDEX('Default Errors'!$F$7:$F$27,MATCH(C42&amp;D42,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>5.8152003828784701E-2</v>
+      </c>
+      <c r="P42" s="9">
+        <f t="shared" ref="P42:P61" si="13">M42/N42</f>
+        <v>1.3356748853859927E-2</v>
+      </c>
+      <c r="Q42" s="9">
+        <f t="shared" ref="Q42:Q61" si="14">SQRT(P42)</f>
+        <v>0.11557140153974048</v>
+      </c>
+      <c r="R42" s="9">
+        <f t="shared" ref="R42:R61" si="15">M42/O42</f>
+        <v>3.4324551238421777E-2</v>
+      </c>
+      <c r="S42" s="9">
+        <f t="shared" ref="S42:S61" si="16">SQRT(R42)</f>
+        <v>0.18526886203143197</v>
+      </c>
       <c r="U42" s="12"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>3</v>
+      </c>
+      <c r="B43" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C43" s="1">
+        <v>16</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
+      <c r="E43" s="4">
+        <v>50</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G43" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H43" s="4">
+        <v>42</v>
+      </c>
+      <c r="I43" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J43" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K43" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="L43" s="14">
+        <v>2.3148148148148146E-4</v>
+      </c>
+      <c r="M43" s="8">
+        <v>3.4603751124252097E-2</v>
+      </c>
+      <c r="N43" s="25">
+        <f t="array" ref="N43">INDEX('Default Errors'!$E$7:$E$27,MATCH(C43&amp;D43,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.148499599467802</v>
+      </c>
+      <c r="O43" s="25">
+        <f t="array" ref="O43">INDEX('Default Errors'!$F$7:$F$27,MATCH(C43&amp;D43,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.11889890066757899</v>
+      </c>
+      <c r="P43" s="9">
+        <f t="shared" si="13"/>
+        <v>0.23302252159781048</v>
+      </c>
+      <c r="Q43" s="9">
+        <f t="shared" si="14"/>
+        <v>0.48272406362000486</v>
+      </c>
+      <c r="R43" s="9">
+        <f t="shared" si="15"/>
+        <v>0.29103508047562415</v>
+      </c>
+      <c r="S43" s="9">
+        <f t="shared" si="16"/>
+        <v>0.53947667278170996</v>
+      </c>
       <c r="U43" s="12"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>4</v>
+      </c>
+      <c r="B44" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C44" s="1">
+        <v>32</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" s="4">
+        <v>200</v>
+      </c>
+      <c r="F44" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G44" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H44" s="4">
+        <v>40</v>
+      </c>
+      <c r="I44" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J44" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="K44" s="16">
+        <v>5000</v>
+      </c>
+      <c r="L44" s="14">
+        <v>1.5162037037037036E-3</v>
+      </c>
+      <c r="M44" s="8">
+        <v>8.5608063744124802E-2</v>
+      </c>
+      <c r="N44" s="25">
+        <f t="array" ref="N44">INDEX('Default Errors'!$E$7:$E$27,MATCH(C44&amp;D44,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.14549183579793001</v>
+      </c>
+      <c r="O44" s="25">
+        <f t="array" ref="O44">INDEX('Default Errors'!$F$7:$F$27,MATCH(C44&amp;D44,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.14159938339096101</v>
+      </c>
+      <c r="P44" s="9">
+        <f t="shared" si="13"/>
+        <v>0.58840458830297326</v>
+      </c>
+      <c r="Q44" s="9">
+        <f t="shared" si="14"/>
+        <v>0.76707534721367054</v>
+      </c>
+      <c r="R44" s="9">
+        <f t="shared" si="15"/>
+        <v>0.60457935404815888</v>
+      </c>
+      <c r="S44" s="9">
+        <f t="shared" si="16"/>
+        <v>0.7775470108283864</v>
+      </c>
       <c r="U44" s="12"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>5</v>
+      </c>
+      <c r="B45" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C45" s="1">
+        <v>64</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="4">
+        <v>400</v>
+      </c>
+      <c r="F45" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G45" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H45" s="4">
+        <v>39</v>
+      </c>
+      <c r="I45" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J45" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K45" s="16">
+        <v>50000</v>
+      </c>
+      <c r="L45" s="14">
+        <v>1.3958333333333335E-2</v>
+      </c>
+      <c r="M45" s="8">
+        <v>0.129747710464202</v>
+      </c>
+      <c r="N45" s="25">
+        <f t="array" ref="N45">INDEX('Default Errors'!$E$7:$E$27,MATCH(C45&amp;D45,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.144625530038068</v>
+      </c>
+      <c r="O45" s="25">
+        <f t="array" ref="O45">INDEX('Default Errors'!$F$7:$F$27,MATCH(C45&amp;D45,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.14637915004454899</v>
+      </c>
+      <c r="P45" s="9">
+        <f t="shared" si="13"/>
+        <v>0.89712867728159829</v>
+      </c>
+      <c r="Q45" s="9">
+        <f t="shared" si="14"/>
+        <v>0.94716876916503023</v>
+      </c>
+      <c r="R45" s="9">
+        <f t="shared" si="15"/>
+        <v>0.88638108927886672</v>
+      </c>
+      <c r="S45" s="9">
+        <f t="shared" si="16"/>
+        <v>0.94147814062720903</v>
+      </c>
       <c r="U45" s="12"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>6</v>
+      </c>
+      <c r="B46" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C46" s="1">
+        <v>128</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
+      <c r="E46" s="4">
+        <v>200</v>
+      </c>
+      <c r="F46" s="4">
+        <v>3</v>
+      </c>
+      <c r="G46" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H46" s="4">
+        <v>41</v>
+      </c>
+      <c r="I46" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J46" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K46" s="16">
+        <v>5000</v>
+      </c>
+      <c r="L46" s="14">
+        <v>3.8402777777777779E-2</v>
+      </c>
+      <c r="M46" s="8">
+        <v>0.15391466481192201</v>
+      </c>
+      <c r="N46" s="25">
+        <f t="array" ref="N46">INDEX('Default Errors'!$E$7:$E$27,MATCH(C46&amp;D46,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.146507455962258</v>
+      </c>
+      <c r="O46" s="25">
+        <f t="array" ref="O46">INDEX('Default Errors'!$F$7:$F$27,MATCH(C46&amp;D46,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.14718499491680501</v>
+      </c>
+      <c r="P46" s="9">
+        <f t="shared" si="13"/>
+        <v>1.0505585794321088</v>
+      </c>
+      <c r="Q46" s="9">
+        <f t="shared" si="14"/>
+        <v>1.0249675992108769</v>
+      </c>
+      <c r="R46" s="9">
+        <f t="shared" si="15"/>
+        <v>1.0457225269391142</v>
+      </c>
+      <c r="S46" s="9">
+        <f t="shared" si="16"/>
+        <v>1.0226057534255879</v>
+      </c>
       <c r="U46" s="12"/>
     </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>7</v>
+      </c>
+      <c r="B47" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C47" s="1">
+        <v>4</v>
+      </c>
+      <c r="D47" s="1">
+        <v>2</v>
+      </c>
+      <c r="E47" s="4">
+        <v>400</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="G47" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="H47" s="4">
+        <v>41</v>
+      </c>
+      <c r="I47" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J47" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K47" s="16">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L47" s="14">
+        <v>4.6296296296296294E-5</v>
+      </c>
+      <c r="M47" s="22">
+        <v>4.7599406016720803E-5</v>
+      </c>
+      <c r="N47" s="25">
+        <f t="array" ref="N47">INDEX('Default Errors'!$E$7:$E$27,MATCH(C47&amp;D47,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.148834244797691</v>
+      </c>
+      <c r="O47" s="25">
+        <f t="array" ref="O47">INDEX('Default Errors'!$F$7:$F$27,MATCH(C47&amp;D47,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>1.8661389182894901E-2</v>
+      </c>
+      <c r="P47" s="9">
+        <f t="shared" si="13"/>
+        <v>3.1981487917261402E-4</v>
+      </c>
+      <c r="Q47" s="9">
+        <f t="shared" si="14"/>
+        <v>1.7883368787021476E-2</v>
+      </c>
+      <c r="R47" s="9">
+        <f t="shared" si="15"/>
+        <v>2.5506893163318514E-3</v>
+      </c>
+      <c r="S47" s="9">
+        <f t="shared" si="16"/>
+        <v>5.0504349479345352E-2</v>
+      </c>
+    </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>8</v>
+      </c>
+      <c r="B48" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C48" s="1">
+        <v>8</v>
+      </c>
+      <c r="D48" s="1">
+        <v>2</v>
+      </c>
+      <c r="E48" s="4">
+        <v>400</v>
+      </c>
+      <c r="F48" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G48" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H48" s="4">
+        <v>41</v>
+      </c>
+      <c r="I48" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J48" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K48" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="L48" s="14">
+        <v>1.6203703703703703E-4</v>
+      </c>
+      <c r="M48" s="8">
+        <v>1.9960414350517698E-3</v>
+      </c>
+      <c r="N48" s="25">
+        <f t="array" ref="N48">INDEX('Default Errors'!$E$7:$E$27,MATCH(C48&amp;D48,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.14944066530540401</v>
+      </c>
+      <c r="O48" s="25">
+        <f t="array" ref="O48">INDEX('Default Errors'!$F$7:$F$27,MATCH(C48&amp;D48,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>5.8152003828784701E-2</v>
+      </c>
+      <c r="P48" s="9">
+        <f t="shared" si="13"/>
+        <v>1.3356748853951937E-2</v>
+      </c>
+      <c r="Q48" s="9">
+        <f t="shared" si="14"/>
+        <v>0.11557140154013854</v>
+      </c>
+      <c r="R48" s="9">
+        <f t="shared" si="15"/>
+        <v>3.4324551238658227E-2</v>
+      </c>
+      <c r="S48" s="9">
+        <f t="shared" si="16"/>
+        <v>0.1852688620320701</v>
+      </c>
       <c r="U48" s="12"/>
     </row>
-    <row r="49" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>9</v>
+      </c>
+      <c r="B49" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C49" s="1">
+        <v>16</v>
+      </c>
+      <c r="D49" s="1">
+        <v>2</v>
+      </c>
+      <c r="E49" s="4">
+        <v>50</v>
+      </c>
+      <c r="F49" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G49" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H49" s="4">
+        <v>42</v>
+      </c>
+      <c r="I49" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J49" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K49" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="L49" s="14">
+        <v>2.3148148148148146E-4</v>
+      </c>
+      <c r="M49" s="8">
+        <v>3.4603751124252097E-2</v>
+      </c>
+      <c r="N49" s="25">
+        <f t="array" ref="N49">INDEX('Default Errors'!$E$7:$E$27,MATCH(C49&amp;D49,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.148499599467802</v>
+      </c>
+      <c r="O49" s="25">
+        <f t="array" ref="O49">INDEX('Default Errors'!$F$7:$F$27,MATCH(C49&amp;D49,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.11889890066757899</v>
+      </c>
+      <c r="P49" s="9">
+        <f t="shared" si="13"/>
+        <v>0.23302252159781048</v>
+      </c>
+      <c r="Q49" s="9">
+        <f t="shared" si="14"/>
+        <v>0.48272406362000486</v>
+      </c>
+      <c r="R49" s="9">
+        <f t="shared" si="15"/>
+        <v>0.29103508047562415</v>
+      </c>
+      <c r="S49" s="9">
+        <f t="shared" si="16"/>
+        <v>0.53947667278170996</v>
+      </c>
       <c r="U49" s="12"/>
     </row>
-    <row r="50" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>10</v>
+      </c>
+      <c r="B50" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C50" s="1">
+        <v>32</v>
+      </c>
+      <c r="D50" s="1">
+        <v>2</v>
+      </c>
+      <c r="E50" s="4">
+        <v>200</v>
+      </c>
+      <c r="F50" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G50" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H50" s="4">
+        <v>40</v>
+      </c>
+      <c r="I50" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J50" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="K50" s="16">
+        <v>5000</v>
+      </c>
+      <c r="L50" s="14">
+        <v>1.5856481481481479E-3</v>
+      </c>
+      <c r="M50" s="8">
+        <v>8.5608063744124802E-2</v>
+      </c>
+      <c r="N50" s="25">
+        <f t="array" ref="N50">INDEX('Default Errors'!$E$7:$E$27,MATCH(C50&amp;D50,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.14549183579793001</v>
+      </c>
+      <c r="O50" s="25">
+        <f t="array" ref="O50">INDEX('Default Errors'!$F$7:$F$27,MATCH(C50&amp;D50,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.14159938339096101</v>
+      </c>
+      <c r="P50" s="9">
+        <f t="shared" si="13"/>
+        <v>0.58840458830297326</v>
+      </c>
+      <c r="Q50" s="9">
+        <f t="shared" si="14"/>
+        <v>0.76707534721367054</v>
+      </c>
+      <c r="R50" s="9">
+        <f t="shared" si="15"/>
+        <v>0.60457935404815888</v>
+      </c>
+      <c r="S50" s="9">
+        <f t="shared" si="16"/>
+        <v>0.7775470108283864</v>
+      </c>
       <c r="U50" s="12"/>
     </row>
-    <row r="51" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>11</v>
+      </c>
+      <c r="B51" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C51" s="1">
+        <v>64</v>
+      </c>
+      <c r="D51" s="1">
+        <v>2</v>
+      </c>
+      <c r="E51" s="4">
+        <v>400</v>
+      </c>
+      <c r="F51" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G51" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H51" s="4">
+        <v>39</v>
+      </c>
+      <c r="I51" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J51" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K51" s="16">
+        <v>50000</v>
+      </c>
+      <c r="L51" s="14">
+        <v>1.2893518518518519E-2</v>
+      </c>
+      <c r="M51" s="8">
+        <v>0.129747710464202</v>
+      </c>
+      <c r="N51" s="25">
+        <f t="array" ref="N51">INDEX('Default Errors'!$E$7:$E$27,MATCH(C51&amp;D51,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.144625530038068</v>
+      </c>
+      <c r="O51" s="25">
+        <f t="array" ref="O51">INDEX('Default Errors'!$F$7:$F$27,MATCH(C51&amp;D51,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.14637915004454899</v>
+      </c>
+      <c r="P51" s="9">
+        <f t="shared" si="13"/>
+        <v>0.89712867728159829</v>
+      </c>
+      <c r="Q51" s="9">
+        <f t="shared" si="14"/>
+        <v>0.94716876916503023</v>
+      </c>
+      <c r="R51" s="9">
+        <f t="shared" si="15"/>
+        <v>0.88638108927886672</v>
+      </c>
+      <c r="S51" s="9">
+        <f t="shared" si="16"/>
+        <v>0.94147814062720903</v>
+      </c>
       <c r="U51" s="12"/>
     </row>
-    <row r="52" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>12</v>
+      </c>
+      <c r="B52" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C52" s="1">
+        <v>128</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2</v>
+      </c>
+      <c r="E52" s="4">
+        <v>200</v>
+      </c>
+      <c r="F52" s="4">
+        <v>3</v>
+      </c>
+      <c r="G52" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H52" s="4">
+        <v>41</v>
+      </c>
+      <c r="I52" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J52" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K52" s="16">
+        <v>5000</v>
+      </c>
+      <c r="L52" s="14">
+        <v>3.8078703703703705E-2</v>
+      </c>
+      <c r="M52" s="8">
+        <v>0.15391466481192201</v>
+      </c>
+      <c r="N52" s="25">
+        <f t="array" ref="N52">INDEX('Default Errors'!$E$7:$E$27,MATCH(C52&amp;D52,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.146507455962258</v>
+      </c>
+      <c r="O52" s="25">
+        <f t="array" ref="O52">INDEX('Default Errors'!$F$7:$F$27,MATCH(C52&amp;D52,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.14718499491680501</v>
+      </c>
+      <c r="P52" s="9">
+        <f t="shared" si="13"/>
+        <v>1.0505585794321088</v>
+      </c>
+      <c r="Q52" s="9">
+        <f t="shared" si="14"/>
+        <v>1.0249675992108769</v>
+      </c>
+      <c r="R52" s="9">
+        <f t="shared" si="15"/>
+        <v>1.0457225269391142</v>
+      </c>
+      <c r="S52" s="9">
+        <f t="shared" si="16"/>
+        <v>1.0226057534255879</v>
+      </c>
       <c r="U52" s="12"/>
     </row>
-    <row r="53" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>13</v>
+      </c>
+      <c r="B53" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C53" s="1">
+        <v>4</v>
+      </c>
+      <c r="D53" s="1">
+        <v>3</v>
+      </c>
+      <c r="E53" s="4">
+        <v>400</v>
+      </c>
+      <c r="F53" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="G53" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="H53" s="4">
+        <v>41</v>
+      </c>
+      <c r="I53" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J53" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K53" s="16">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L53" s="14">
+        <v>4.6296296296296294E-5</v>
+      </c>
+      <c r="M53" s="22">
+        <v>4.7599406016720803E-5</v>
+      </c>
+      <c r="N53" s="25">
+        <f t="array" ref="N53">INDEX('Default Errors'!$E$7:$E$27,MATCH(C53&amp;D53,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.148834244797691</v>
+      </c>
+      <c r="O53" s="25">
+        <f t="array" ref="O53">INDEX('Default Errors'!$F$7:$F$27,MATCH(C53&amp;D53,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>1.8661389182894901E-2</v>
+      </c>
+      <c r="P53" s="9">
+        <f t="shared" si="13"/>
+        <v>3.1981487917261402E-4</v>
+      </c>
+      <c r="Q53" s="9">
+        <f t="shared" si="14"/>
+        <v>1.7883368787021476E-2</v>
+      </c>
+      <c r="R53" s="9">
+        <f t="shared" si="15"/>
+        <v>2.5506893163318514E-3</v>
+      </c>
+      <c r="S53" s="9">
+        <f t="shared" si="16"/>
+        <v>5.0504349479345352E-2</v>
+      </c>
       <c r="U53" s="12"/>
     </row>
-    <row r="54" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>14</v>
+      </c>
+      <c r="B54" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C54" s="1">
+        <v>8</v>
+      </c>
+      <c r="D54" s="1">
+        <v>3</v>
+      </c>
+      <c r="E54" s="4">
+        <v>400</v>
+      </c>
+      <c r="F54" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G54" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H54" s="4">
+        <v>41</v>
+      </c>
+      <c r="I54" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J54" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K54" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="L54" s="14">
+        <v>1.7361111111111112E-4</v>
+      </c>
+      <c r="M54" s="8">
+        <v>1.9960414350355298E-3</v>
+      </c>
+      <c r="N54" s="25">
+        <f t="array" ref="N54">INDEX('Default Errors'!$E$7:$E$27,MATCH(C54&amp;D54,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.14944066530540401</v>
+      </c>
+      <c r="O54" s="25">
+        <f t="array" ref="O54">INDEX('Default Errors'!$F$7:$F$27,MATCH(C54&amp;D54,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>5.8152003828784701E-2</v>
+      </c>
+      <c r="P54" s="9">
+        <f t="shared" si="13"/>
+        <v>1.3356748853843263E-2</v>
+      </c>
+      <c r="Q54" s="9">
+        <f t="shared" si="14"/>
+        <v>0.11557140153966838</v>
+      </c>
+      <c r="R54" s="9">
+        <f t="shared" si="15"/>
+        <v>3.4324551238378957E-2</v>
+      </c>
+      <c r="S54" s="9">
+        <f t="shared" si="16"/>
+        <v>0.18526886203131643</v>
+      </c>
       <c r="U54" s="12"/>
     </row>
-    <row r="55" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>15</v>
+      </c>
+      <c r="B55" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C55" s="1">
+        <v>16</v>
+      </c>
+      <c r="D55" s="1">
+        <v>3</v>
+      </c>
+      <c r="E55" s="4">
+        <v>50</v>
+      </c>
+      <c r="F55" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G55" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H55" s="4">
+        <v>42</v>
+      </c>
+      <c r="I55" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J55" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K55" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="L55" s="14">
+        <v>2.5462962962962961E-4</v>
+      </c>
+      <c r="M55" s="8">
+        <v>3.4603751124252097E-2</v>
+      </c>
+      <c r="N55" s="25">
+        <f t="array" ref="N55">INDEX('Default Errors'!$E$7:$E$27,MATCH(C55&amp;D55,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.148499599467802</v>
+      </c>
+      <c r="O55" s="25">
+        <f t="array" ref="O55">INDEX('Default Errors'!$F$7:$F$27,MATCH(C55&amp;D55,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.11889890066757899</v>
+      </c>
+      <c r="P55" s="9">
+        <f t="shared" si="13"/>
+        <v>0.23302252159781048</v>
+      </c>
+      <c r="Q55" s="9">
+        <f t="shared" si="14"/>
+        <v>0.48272406362000486</v>
+      </c>
+      <c r="R55" s="9">
+        <f t="shared" si="15"/>
+        <v>0.29103508047562415</v>
+      </c>
+      <c r="S55" s="9">
+        <f t="shared" si="16"/>
+        <v>0.53947667278170996</v>
+      </c>
       <c r="U55" s="12"/>
     </row>
-    <row r="56" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>16</v>
+      </c>
+      <c r="B56" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C56" s="1">
+        <v>32</v>
+      </c>
+      <c r="D56" s="1">
+        <v>3</v>
+      </c>
+      <c r="E56" s="4">
+        <v>200</v>
+      </c>
+      <c r="F56" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G56" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H56" s="4">
+        <v>40</v>
+      </c>
+      <c r="I56" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J56" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="K56" s="16">
+        <v>5000</v>
+      </c>
+      <c r="L56" s="14">
+        <v>1.5624999999999999E-3</v>
+      </c>
+      <c r="M56" s="8">
+        <v>8.5608063744124802E-2</v>
+      </c>
+      <c r="N56" s="25">
+        <f t="array" ref="N56">INDEX('Default Errors'!$E$7:$E$27,MATCH(C56&amp;D56,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.14549183579793001</v>
+      </c>
+      <c r="O56" s="25">
+        <f t="array" ref="O56">INDEX('Default Errors'!$F$7:$F$27,MATCH(C56&amp;D56,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.14159938339096101</v>
+      </c>
+      <c r="P56" s="9">
+        <f t="shared" si="13"/>
+        <v>0.58840458830297326</v>
+      </c>
+      <c r="Q56" s="9">
+        <f t="shared" si="14"/>
+        <v>0.76707534721367054</v>
+      </c>
+      <c r="R56" s="9">
+        <f t="shared" si="15"/>
+        <v>0.60457935404815888</v>
+      </c>
+      <c r="S56" s="9">
+        <f t="shared" si="16"/>
+        <v>0.7775470108283864</v>
+      </c>
       <c r="U56" s="12"/>
     </row>
-    <row r="57" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>17</v>
+      </c>
+      <c r="B57" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C57" s="1">
+        <v>64</v>
+      </c>
+      <c r="D57" s="1">
+        <v>3</v>
+      </c>
+      <c r="E57" s="4">
+        <v>400</v>
+      </c>
+      <c r="F57" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G57" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H57" s="4">
+        <v>39</v>
+      </c>
+      <c r="I57" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J57" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K57" s="16">
+        <v>50000</v>
+      </c>
+      <c r="L57" s="14">
+        <v>1.2534722222222223E-2</v>
+      </c>
+      <c r="M57" s="8">
+        <v>0.129747710464202</v>
+      </c>
+      <c r="N57" s="25">
+        <f t="array" ref="N57">INDEX('Default Errors'!$E$7:$E$27,MATCH(C57&amp;D57,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.144625530038068</v>
+      </c>
+      <c r="O57" s="25">
+        <f t="array" ref="O57">INDEX('Default Errors'!$F$7:$F$27,MATCH(C57&amp;D57,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.14637915004454899</v>
+      </c>
+      <c r="P57" s="9">
+        <f t="shared" si="13"/>
+        <v>0.89712867728159829</v>
+      </c>
+      <c r="Q57" s="9">
+        <f t="shared" si="14"/>
+        <v>0.94716876916503023</v>
+      </c>
+      <c r="R57" s="9">
+        <f t="shared" si="15"/>
+        <v>0.88638108927886672</v>
+      </c>
+      <c r="S57" s="9">
+        <f t="shared" si="16"/>
+        <v>0.94147814062720903</v>
+      </c>
       <c r="U57" s="12"/>
     </row>
-    <row r="58" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>18</v>
+      </c>
+      <c r="B58" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C58" s="1">
+        <v>128</v>
+      </c>
+      <c r="D58" s="1">
+        <v>3</v>
+      </c>
+      <c r="E58" s="4">
+        <v>200</v>
+      </c>
+      <c r="F58" s="4">
+        <v>3</v>
+      </c>
+      <c r="G58" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H58" s="4">
+        <v>41</v>
+      </c>
+      <c r="I58" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J58" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K58" s="16">
+        <v>5000</v>
+      </c>
+      <c r="L58" s="14">
+        <v>3.8310185185185183E-2</v>
+      </c>
+      <c r="M58" s="8">
+        <v>0.15391466481192201</v>
+      </c>
+      <c r="N58" s="25">
+        <f t="array" ref="N58">INDEX('Default Errors'!$E$7:$E$27,MATCH(C58&amp;D58,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.146507455962258</v>
+      </c>
+      <c r="O58" s="25">
+        <f t="array" ref="O58">INDEX('Default Errors'!$F$7:$F$27,MATCH(C58&amp;D58,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.14718499491680501</v>
+      </c>
+      <c r="P58" s="9">
+        <f t="shared" si="13"/>
+        <v>1.0505585794321088</v>
+      </c>
+      <c r="Q58" s="9">
+        <f t="shared" si="14"/>
+        <v>1.0249675992108769</v>
+      </c>
+      <c r="R58" s="9">
+        <f t="shared" si="15"/>
+        <v>1.0457225269391142</v>
+      </c>
+      <c r="S58" s="9">
+        <f t="shared" si="16"/>
+        <v>1.0226057534255879</v>
+      </c>
       <c r="U58" s="12"/>
     </row>
-    <row r="59" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>19</v>
+      </c>
+      <c r="B59" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C59" s="1">
+        <v>146</v>
+      </c>
+      <c r="D59" s="1">
+        <v>1</v>
+      </c>
+      <c r="E59" s="4">
+        <v>50</v>
+      </c>
+      <c r="F59" s="4">
+        <v>3</v>
+      </c>
+      <c r="G59" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H59" s="4">
+        <v>41</v>
+      </c>
+      <c r="I59" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J59" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="K59" s="16">
+        <v>500</v>
+      </c>
+      <c r="L59" s="14">
+        <v>3.3599537037037039E-2</v>
+      </c>
+      <c r="M59" s="8">
+        <v>0.17220235429966699</v>
+      </c>
+      <c r="N59" s="25">
+        <f t="array" ref="N59">INDEX('Default Errors'!$E$7:$E$27,MATCH(C59&amp;D59,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.14741263428892101</v>
+      </c>
+      <c r="O59" s="25">
+        <f t="array" ref="O59">INDEX('Default Errors'!$F$7:$F$27,MATCH(C59&amp;D59,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.157221673028453</v>
+      </c>
+      <c r="P59" s="9">
+        <f t="shared" si="13"/>
+        <v>1.1681655044720212</v>
+      </c>
+      <c r="Q59" s="9">
+        <f t="shared" si="14"/>
+        <v>1.0808170541178657</v>
+      </c>
+      <c r="R59" s="9">
+        <f t="shared" si="15"/>
+        <v>1.0952838179536666</v>
+      </c>
+      <c r="S59" s="9">
+        <f t="shared" si="16"/>
+        <v>1.0465580815003372</v>
+      </c>
       <c r="U59" s="12"/>
     </row>
-    <row r="60" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>20</v>
+      </c>
+      <c r="B60" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C60" s="1">
+        <v>146</v>
+      </c>
+      <c r="D60" s="1">
+        <v>2</v>
+      </c>
+      <c r="E60" s="4">
+        <v>50</v>
+      </c>
+      <c r="F60" s="4">
+        <v>3</v>
+      </c>
+      <c r="G60" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H60" s="4">
+        <v>41</v>
+      </c>
+      <c r="I60" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J60" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="K60" s="16">
+        <v>500</v>
+      </c>
+      <c r="L60" s="14">
+        <v>3.425925925925926E-2</v>
+      </c>
+      <c r="M60" s="8">
+        <v>0.17358009079287801</v>
+      </c>
+      <c r="N60" s="25">
+        <f t="array" ref="N60">INDEX('Default Errors'!$E$7:$E$27,MATCH(C60&amp;D60,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.14741263428892101</v>
+      </c>
+      <c r="O60" s="25">
+        <f t="array" ref="O60">INDEX('Default Errors'!$F$7:$F$27,MATCH(C60&amp;D60,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.157221673028453</v>
+      </c>
+      <c r="P60" s="9">
+        <f t="shared" si="13"/>
+        <v>1.1775116266674277</v>
+      </c>
+      <c r="Q60" s="9">
+        <f t="shared" si="14"/>
+        <v>1.0851320779828728</v>
+      </c>
+      <c r="R60" s="9">
+        <f t="shared" si="15"/>
+        <v>1.1040468368598557</v>
+      </c>
+      <c r="S60" s="9">
+        <f t="shared" si="16"/>
+        <v>1.0507363307984814</v>
+      </c>
       <c r="U60" s="12"/>
     </row>
-    <row r="61" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>21</v>
+      </c>
+      <c r="B61" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C61" s="1">
+        <v>148</v>
+      </c>
+      <c r="D61" s="1">
+        <v>1</v>
+      </c>
+      <c r="E61" s="4">
+        <v>400</v>
+      </c>
+      <c r="F61" s="4">
+        <v>3</v>
+      </c>
+      <c r="G61" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H61" s="4">
+        <v>39</v>
+      </c>
+      <c r="I61" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J61" s="16">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K61" s="16">
+        <v>500</v>
+      </c>
+      <c r="L61" s="14">
+        <v>0.13192129629629631</v>
+      </c>
+      <c r="M61" s="8">
+        <v>0.18486893039771801</v>
+      </c>
+      <c r="N61" s="25">
+        <f t="array" ref="N61">INDEX('Default Errors'!$E$7:$E$27,MATCH(C61&amp;D61,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.148183907230964</v>
+      </c>
+      <c r="O61" s="25">
+        <f t="array" ref="O61">INDEX('Default Errors'!$F$7:$F$27,MATCH(C61&amp;D61,'Default Errors'!$C$7:$C$27&amp;'Default Errors'!$D$7:$D$27,0))</f>
+        <v>0.15764528369873401</v>
+      </c>
+      <c r="P61" s="9">
+        <f t="shared" si="13"/>
+        <v>1.2475641508735196</v>
+      </c>
+      <c r="Q61" s="9">
+        <f t="shared" si="14"/>
+        <v>1.116944112690299</v>
+      </c>
+      <c r="R61" s="9">
+        <f t="shared" si="15"/>
+        <v>1.1726892556520079</v>
+      </c>
+      <c r="S61" s="9">
+        <f t="shared" si="16"/>
+        <v>1.0829077779995893</v>
+      </c>
       <c r="U61" s="12"/>
     </row>
-    <row r="62" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U62" s="12"/>
     </row>
-    <row r="63" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U63" s="12"/>
     </row>
-    <row r="64" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U64" s="12"/>
     </row>
     <row r="65" spans="21:21" x14ac:dyDescent="0.25">
@@ -48722,14 +51551,14 @@
       </c>
     </row>
     <row r="5" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="J5" s="29" t="s">
+      <c r="F5" s="30"/>
+      <c r="J5" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="29"/>
+      <c r="K5" s="30"/>
     </row>
     <row r="6" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C6" t="s">

</xml_diff>

<commit_message>
feature: added new results
</commit_message>
<xml_diff>
--- a/src/final/inner_prediction/inner_cross_pred_results.xlsx
+++ b/src/final/inner_prediction/inner_cross_pred_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="3" activeTab="7"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="17" r:id="rId1"/>
@@ -44357,8 +44357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S84"/>
   <sheetViews>
-    <sheetView topLeftCell="H43" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46:M66"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47966,8 +47966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:U84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33:M33"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L11" sqref="A11:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48015,8 +48015,12 @@
       <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <f t="shared" ref="A8:M8" si="0">INDEX(A$17:A$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,4),$M$17:$M$999,))</f>
+        <v>1</v>
+      </c>
       <c r="B8" s="7">
-        <f t="shared" ref="B8:M8" si="0">INDEX(B$17:B$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,4),$M$17:$M$999,))</f>
+        <f t="shared" si="0"/>
         <v>15000</v>
       </c>
       <c r="C8" s="7">
@@ -48083,8 +48087,12 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <f t="shared" ref="A9:M9" si="1">INDEX(A$17:A$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,8),$M$17:$M$999,))</f>
+        <v>14</v>
+      </c>
       <c r="B9" s="7">
-        <f t="shared" ref="B9:M9" si="1">INDEX(B$17:B$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,8),$M$17:$M$999,))</f>
+        <f t="shared" si="1"/>
         <v>15000</v>
       </c>
       <c r="C9" s="7">
@@ -48151,8 +48159,12 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <f t="shared" ref="A10:M10" si="2">INDEX(A$17:A$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,16),$M$17:$M$999,))</f>
+        <v>3</v>
+      </c>
       <c r="B10" s="7">
-        <f t="shared" ref="B10:M10" si="2">INDEX(B$17:B$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,16),$M$17:$M$999,))</f>
+        <f t="shared" si="2"/>
         <v>15000</v>
       </c>
       <c r="C10" s="7">
@@ -48220,8 +48232,12 @@
       <c r="U10" s="15"/>
     </row>
     <row r="11" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <f t="shared" ref="A11:M11" si="3">INDEX(A$17:A$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,32),$M$17:$M$999,))</f>
+        <v>4</v>
+      </c>
       <c r="B11" s="7">
-        <f t="shared" ref="B11:M11" si="3">INDEX(B$17:B$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,32),$M$17:$M$999,))</f>
+        <f t="shared" si="3"/>
         <v>15000</v>
       </c>
       <c r="C11" s="7">
@@ -48289,8 +48305,12 @@
       <c r="U11" s="15"/>
     </row>
     <row r="12" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <f t="shared" ref="A12:M12" si="4">INDEX(A$17:A$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,64),$M$17:$M$999,))</f>
+        <v>5</v>
+      </c>
       <c r="B12" s="7">
-        <f t="shared" ref="B12:M12" si="4">INDEX(B$17:B$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,64),$M$17:$M$999,))</f>
+        <f t="shared" si="4"/>
         <v>15000</v>
       </c>
       <c r="C12" s="7">
@@ -48358,8 +48378,12 @@
       <c r="U12" s="15"/>
     </row>
     <row r="13" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <f t="shared" ref="A13:M13" si="5">INDEX(A$17:A$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,128),$M$17:$M$999,))</f>
+        <v>6</v>
+      </c>
       <c r="B13" s="7">
-        <f t="shared" ref="B13:M13" si="5">INDEX(B$17:B$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,128),$M$17:$M$999,))</f>
+        <f t="shared" si="5"/>
         <v>15000</v>
       </c>
       <c r="C13" s="7">
@@ -48427,8 +48451,12 @@
       <c r="U13" s="15"/>
     </row>
     <row r="14" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <f t="shared" ref="A14:M14" si="6">INDEX(A$17:A$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,146),$M$17:$M$999,))</f>
+        <v>19</v>
+      </c>
       <c r="B14" s="7">
-        <f t="shared" ref="B14:M14" si="6">INDEX(B$17:B$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,146),$M$17:$M$999,))</f>
+        <f t="shared" si="6"/>
         <v>15000</v>
       </c>
       <c r="C14" s="7">
@@ -48496,8 +48524,12 @@
       <c r="U14" s="15"/>
     </row>
     <row r="15" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <f t="shared" ref="A15:M15" si="7">INDEX(A$17:A$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,148),$M$17:$M$999,))</f>
+        <v>21</v>
+      </c>
       <c r="B15" s="7">
-        <f t="shared" ref="B15:M15" si="7">INDEX(B$17:B$999,MATCH(_xlfn.MINIFS($M$17:$M$999,$C$17:$C$999,148),$M$17:$M$999,))</f>
+        <f t="shared" si="7"/>
         <v>15000</v>
       </c>
       <c r="C15" s="7">

</xml_diff>